<commit_message>
more skills added to units
</commit_message>
<xml_diff>
--- a/Documentation.xlsx
+++ b/Documentation.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Overview" sheetId="2" r:id="rId1"/>
     <sheet name="Units" sheetId="4" r:id="rId2"/>
-    <sheet name="Skills-Overview" sheetId="9" r:id="rId3"/>
+    <sheet name="Skills-Overview" sheetId="9" state="hidden" r:id="rId3"/>
     <sheet name="Skills" sheetId="7" r:id="rId4"/>
     <sheet name="Weapons" sheetId="1" r:id="rId5"/>
     <sheet name="Weapons-Overview" sheetId="3" r:id="rId6"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="693">
   <si>
     <t>physical</t>
   </si>
@@ -1370,9 +1370,6 @@
     <t>Lunar Blessing</t>
   </si>
   <si>
-    <t>Heal target ally.</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -1556,9 +1553,6 @@
     <t>Heal target ally to full health. Reduce unit's health to 1.</t>
   </si>
   <si>
-    <t>Meteor</t>
-  </si>
-  <si>
     <t>Deals damage to three random enemies.</t>
   </si>
   <si>
@@ -1796,9 +1790,6 @@
     <t>Eathquake</t>
   </si>
   <si>
-    <t>Damages all enemies and has a chance (15%) to Stun(1) enemies.</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
@@ -1844,9 +1835,6 @@
     <t>Envenom</t>
   </si>
   <si>
-    <t>All damage dealt by unit inflicts Bleed(2) on target.</t>
-  </si>
-  <si>
     <t>Dark Priest</t>
   </si>
   <si>
@@ -1887,6 +1875,240 @@
   </si>
   <si>
     <t>Inflicts Bleed(2) and grants all allies a shield for 5% of units current health.</t>
+  </si>
+  <si>
+    <t>Black Mark</t>
+  </si>
+  <si>
+    <t>On death, inflicts Cursed(2) on all enemies. (Cursed: target takes double damage from any source and removes Cursed.)</t>
+  </si>
+  <si>
+    <t>Gouge</t>
+  </si>
+  <si>
+    <t>Bind: Reduces target speed by 40%.</t>
+  </si>
+  <si>
+    <t>Curse: Next damaging skill/ability/weapon does double damage and consumes the Curse marker.</t>
+  </si>
+  <si>
+    <t>Comet Storm</t>
+  </si>
+  <si>
+    <t>Inflicts Burn(4) on target.</t>
+  </si>
+  <si>
+    <t>Meteor Strike</t>
+  </si>
+  <si>
+    <t>Enchanted Horn</t>
+  </si>
+  <si>
+    <t>[Guardian Angel]</t>
+  </si>
+  <si>
+    <t>Warrior Gem</t>
+  </si>
+  <si>
+    <t>Arcane Gem</t>
+  </si>
+  <si>
+    <t>Gain Str/Amr +20.</t>
+  </si>
+  <si>
+    <t>Gain Fcs/Res +20.</t>
+  </si>
+  <si>
+    <t>Immune to Poison. Increases damage dealth to Poisoned targets (20%).</t>
+  </si>
+  <si>
+    <t>Damages all enemies and has a chance (15%) to inflict Stun(1) on each target.</t>
+  </si>
+  <si>
+    <t>Thundering Blow</t>
+  </si>
+  <si>
+    <t>Has a 20% chance to inflict Sleep(4) on target whenever unit attacks.</t>
+  </si>
+  <si>
+    <t>Scuttle</t>
+  </si>
+  <si>
+    <t>Has a chance (50%) to inflict Poison(4) on target.</t>
+  </si>
+  <si>
+    <t>High critical hit chance doubled, 90% against Burned targets).</t>
+  </si>
+  <si>
+    <t>Adaptive Mind</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>Deals more damage the less health target has.</t>
+  </si>
+  <si>
+    <t>All damage dealt by unit inflicts Poison(2) on target.</t>
+  </si>
+  <si>
+    <t>Poison: Target takes damage = 15% of unit's Strength/Focus (whichever is higher).</t>
+  </si>
+  <si>
+    <t>Burn: Target takes damage = 10% of their max health at the end of every round.</t>
+  </si>
+  <si>
+    <t>Power Chain</t>
+  </si>
+  <si>
+    <t>Inflicts Bind(1) on target. (Bind: decreases target's speed by 40%.)</t>
+  </si>
+  <si>
+    <t>Encase</t>
+  </si>
+  <si>
+    <t>self</t>
+  </si>
+  <si>
+    <t>Increases Amr/Res.</t>
+  </si>
+  <si>
+    <t>Increase all allies Str/Fcs/Spd.</t>
+  </si>
+  <si>
+    <t>Heal target ally (100% unit's Focus).</t>
+  </si>
+  <si>
+    <t>Anarchy</t>
+  </si>
+  <si>
+    <t>Randomly increases 3 allies' Spd/Str/Fcs.</t>
+  </si>
+  <si>
+    <t>Timber</t>
+  </si>
+  <si>
+    <t>Hits all units in a row</t>
+  </si>
+  <si>
+    <t>Noble Smite</t>
+  </si>
+  <si>
+    <t>Does increased damage to Stunned enemies.</t>
+  </si>
+  <si>
+    <t>Immune to damage over time effects like Bleed, Burn, and Poison.</t>
+  </si>
+  <si>
+    <t>Has a 50% chance to inflict Stun(1) or Silence(1) on target.</t>
+  </si>
+  <si>
+    <t>Increasese unit's Str/Fcs/Spd.</t>
+  </si>
+  <si>
+    <t>Shadow Swap</t>
+  </si>
+  <si>
+    <t>Wildfire</t>
+  </si>
+  <si>
+    <t>Hits 4 random enemies.</t>
+  </si>
+  <si>
+    <t>Sacrifice</t>
+  </si>
+  <si>
+    <t>Poison Barbs</t>
+  </si>
+  <si>
+    <t>Inflicts Poison(2) on target.</t>
+  </si>
+  <si>
+    <t>Black Oath</t>
+  </si>
+  <si>
+    <t>Vile Penance</t>
+  </si>
+  <si>
+    <t>Deal (20% of current Health) damage to unit after combat.</t>
+  </si>
+  <si>
+    <t>Viper's Affliction</t>
+  </si>
+  <si>
+    <t>Plaguebringer</t>
+  </si>
+  <si>
+    <t>On death, inflict Poison(8) on all enemies.</t>
+  </si>
+  <si>
+    <t>Soul Charm</t>
+  </si>
+  <si>
+    <t>Lower all enemies Str/Fcs (5%).</t>
+  </si>
+  <si>
+    <t>Torment</t>
+  </si>
+  <si>
+    <t>Nullify</t>
+  </si>
+  <si>
+    <t>Remove all stat bonuses from target.</t>
+  </si>
+  <si>
+    <t>Hasten</t>
+  </si>
+  <si>
+    <t>Increase target Speed (50%).</t>
+  </si>
+  <si>
+    <t>Annihilate</t>
+  </si>
+  <si>
+    <t>Deal (20% current health) damage to unit. Heal target ally for twice damage dealt.</t>
+  </si>
+  <si>
+    <t>Aether Blessing</t>
+  </si>
+  <si>
+    <t>Void Blessing</t>
+  </si>
+  <si>
+    <t>Converts all stat decreases into increases.</t>
+  </si>
+  <si>
+    <t>Spiritual Affliction</t>
+  </si>
+  <si>
+    <t>Empty Mind</t>
+  </si>
+  <si>
+    <t>Immune to all stat changes.</t>
+  </si>
+  <si>
+    <t>Protect</t>
+  </si>
+  <si>
+    <t>Shield target ally (60% Focus).</t>
+  </si>
+  <si>
+    <t>Taunt</t>
+  </si>
+  <si>
+    <t>Lower target Amr/Res (20%).</t>
+  </si>
+  <si>
+    <t>Psychic Shackle</t>
+  </si>
+  <si>
+    <t>Nightmare</t>
+  </si>
+  <si>
+    <t>Doesl double damage to sleeping target.</t>
+  </si>
+  <si>
+    <t>Puncture</t>
   </si>
 </sst>
 </file>
@@ -2337,7 +2559,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>103663</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1628775" cy="352469"/>
@@ -2845,7 +3067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H96"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -3410,8 +3632,8 @@
   <dimension ref="A1:R128"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N20" sqref="N20"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K20" sqref="K20:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3456,19 +3678,19 @@
         <v>177</v>
       </c>
       <c r="K1" s="31" t="s">
+        <v>463</v>
+      </c>
+      <c r="L1" s="31" t="s">
         <v>464</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="M1" s="31" t="s">
         <v>465</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="N1" s="31" t="s">
         <v>466</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="O1" s="31" t="s">
         <v>467</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>468</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>169</v>
@@ -3606,7 +3828,7 @@
         <v>278</v>
       </c>
       <c r="O5" s="74" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -3674,8 +3896,11 @@
         <f t="shared" si="0"/>
         <v>208</v>
       </c>
+      <c r="N7" s="74" t="s">
+        <v>642</v>
+      </c>
       <c r="O7" s="71" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -3843,7 +4068,7 @@
         <v>257</v>
       </c>
       <c r="O12" s="74" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -3879,7 +4104,10 @@
         <v>258</v>
       </c>
       <c r="N13" s="74" t="s">
-        <v>515</v>
+        <v>513</v>
+      </c>
+      <c r="O13" s="74" t="s">
+        <v>642</v>
       </c>
       <c r="P13" t="s">
         <v>293</v>
@@ -3953,6 +4181,12 @@
         <f t="shared" si="0"/>
         <v>334</v>
       </c>
+      <c r="K15" s="69" t="s">
+        <v>555</v>
+      </c>
+      <c r="O15" s="69" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" t="s">
@@ -3986,8 +4220,11 @@
         <f t="shared" si="0"/>
         <v>327</v>
       </c>
+      <c r="K16" s="69" t="s">
+        <v>555</v>
+      </c>
       <c r="O16" s="69" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -4022,6 +4259,9 @@
         <f>SUM(D17:I17)</f>
         <v>355</v>
       </c>
+      <c r="K17" s="69" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" t="s">
@@ -4122,16 +4362,19 @@
         <v>356</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L20" s="75" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
+      </c>
+      <c r="N20" s="69" t="s">
+        <v>637</v>
       </c>
       <c r="O20" s="69" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -4167,19 +4410,19 @@
         <v>356</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L21" s="75" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="N21" s="69" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="O21" s="69" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -4215,7 +4458,7 @@
         <v>392</v>
       </c>
       <c r="O22" s="71" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -4251,7 +4494,7 @@
         <v>434</v>
       </c>
       <c r="N23" s="71" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -4287,7 +4530,7 @@
         <v>390</v>
       </c>
       <c r="N24" s="71" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -4322,8 +4565,20 @@
         <f t="shared" si="0"/>
         <v>271</v>
       </c>
+      <c r="K26" s="70" t="s">
+        <v>633</v>
+      </c>
+      <c r="L26" s="57" t="s">
+        <v>532</v>
+      </c>
+      <c r="M26" s="69" t="s">
+        <v>452</v>
+      </c>
       <c r="N26" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
+      </c>
+      <c r="O26" s="70" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -4358,6 +4613,15 @@
         <f t="shared" si="0"/>
         <v>257</v>
       </c>
+      <c r="K27" s="70" t="s">
+        <v>617</v>
+      </c>
+      <c r="M27" s="70" t="s">
+        <v>533</v>
+      </c>
+      <c r="O27" s="69" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" t="s">
@@ -4391,6 +4655,9 @@
         <f t="shared" si="0"/>
         <v>267</v>
       </c>
+      <c r="K28" s="70" t="s">
+        <v>533</v>
+      </c>
       <c r="P28" t="s">
         <v>348</v>
       </c>
@@ -4427,6 +4694,9 @@
         <f t="shared" si="0"/>
         <v>281</v>
       </c>
+      <c r="K29" s="70" t="s">
+        <v>533</v>
+      </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" t="s">
@@ -4460,6 +4730,12 @@
         <f t="shared" si="0"/>
         <v>315</v>
       </c>
+      <c r="K30" s="70" t="s">
+        <v>533</v>
+      </c>
+      <c r="M30" s="70" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" t="s">
@@ -4493,8 +4769,14 @@
         <f t="shared" si="0"/>
         <v>285</v>
       </c>
+      <c r="K31" s="70" t="s">
+        <v>533</v>
+      </c>
       <c r="L31" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
+      </c>
+      <c r="N31" s="70" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -4529,8 +4811,14 @@
         <f t="shared" si="0"/>
         <v>264</v>
       </c>
+      <c r="K32" s="70" t="s">
+        <v>533</v>
+      </c>
       <c r="L32" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
+      </c>
+      <c r="M32" s="70" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -4565,6 +4853,12 @@
         <f>SUM(D33:I33)</f>
         <v>274</v>
       </c>
+      <c r="K33" s="70" t="s">
+        <v>617</v>
+      </c>
+      <c r="L33" s="70" t="s">
+        <v>533</v>
+      </c>
       <c r="P33" t="s">
         <v>254</v>
       </c>
@@ -4601,6 +4895,12 @@
         <f t="shared" si="0"/>
         <v>373</v>
       </c>
+      <c r="K34" s="70" t="s">
+        <v>644</v>
+      </c>
+      <c r="N34" s="74" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="35" spans="1:16">
       <c r="A35" t="s">
@@ -4634,6 +4934,9 @@
         <f t="shared" si="0"/>
         <v>352</v>
       </c>
+      <c r="L35" s="70" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="36" spans="1:16">
       <c r="A36" t="s">
@@ -4994,7 +5297,7 @@
         <v>189</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D46" s="28">
         <v>99</v>
@@ -5019,13 +5322,16 @@
         <v>494</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="L46" s="74" t="s">
-        <v>560</v>
+        <v>573</v>
+      </c>
+      <c r="L46" s="70" t="s">
+        <v>644</v>
+      </c>
+      <c r="M46" s="74" t="s">
+        <v>558</v>
       </c>
       <c r="N46" s="70" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -5036,7 +5342,7 @@
         <v>189</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D47" s="28">
         <v>99</v>
@@ -5061,10 +5367,10 @@
         <v>480</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="L47" s="74" t="s">
-        <v>560</v>
+        <v>573</v>
+      </c>
+      <c r="M47" s="74" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -5075,7 +5381,7 @@
         <v>189</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D48" s="28">
         <v>110</v>
@@ -5100,16 +5406,19 @@
         <v>551</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="L48" s="74" t="s">
-        <v>560</v>
-      </c>
-      <c r="M48" s="4" t="s">
-        <v>613</v>
+        <v>573</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="M48" s="74" t="s">
+        <v>558</v>
       </c>
       <c r="N48" s="74" t="s">
-        <v>573</v>
+        <v>571</v>
+      </c>
+      <c r="O48" s="72" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="50" spans="1:18">
@@ -5180,6 +5489,9 @@
         <f t="shared" si="0"/>
         <v>392</v>
       </c>
+      <c r="K51" s="69" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="52" spans="1:18">
       <c r="A52" t="s">
@@ -5214,7 +5526,7 @@
         <v>397</v>
       </c>
       <c r="O52" s="74" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="53" spans="1:18">
@@ -5250,7 +5562,7 @@
         <v>346</v>
       </c>
       <c r="K53" s="71" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="54" spans="1:18">
@@ -5285,6 +5597,12 @@
         <f t="shared" ref="J54:J60" si="2">SUM(D54:I54)</f>
         <v>366</v>
       </c>
+      <c r="K54" s="69" t="s">
+        <v>555</v>
+      </c>
+      <c r="O54" s="72" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="55" spans="1:18">
       <c r="A55" t="s">
@@ -5318,6 +5636,12 @@
         <f t="shared" si="2"/>
         <v>338</v>
       </c>
+      <c r="K55" s="69" t="s">
+        <v>555</v>
+      </c>
+      <c r="O55" s="72" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="56" spans="1:18">
       <c r="A56" t="s">
@@ -5351,6 +5675,12 @@
         <f t="shared" si="2"/>
         <v>295</v>
       </c>
+      <c r="K56" s="69" t="s">
+        <v>555</v>
+      </c>
+      <c r="O56" s="72" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="57" spans="1:18">
       <c r="A57" t="s">
@@ -5385,7 +5715,7 @@
         <v>401</v>
       </c>
       <c r="M57" s="71" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P57" t="s">
         <v>288</v>
@@ -5463,7 +5793,7 @@
         <v>333</v>
       </c>
       <c r="M59" s="71" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P59" t="s">
         <v>288</v>
@@ -5505,7 +5835,7 @@
         <v>443</v>
       </c>
       <c r="K60" s="71" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P60" t="s">
         <v>289</v>
@@ -5543,8 +5873,11 @@
         <f t="shared" ref="J61:J66" si="3">SUM(D61:I61)</f>
         <v>451</v>
       </c>
+      <c r="K61" s="70" t="s">
+        <v>644</v>
+      </c>
       <c r="M61" s="71" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="62" spans="1:18">
@@ -5580,7 +5913,7 @@
         <v>494</v>
       </c>
       <c r="K62" s="71" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P62" t="s">
         <v>295</v>
@@ -5619,7 +5952,7 @@
         <v>445</v>
       </c>
       <c r="K63" s="73" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="64" spans="1:18">
@@ -5655,7 +5988,7 @@
         <v>428</v>
       </c>
       <c r="N64" s="71" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="P64" t="s">
         <v>414</v>
@@ -5694,7 +6027,7 @@
         <v>381</v>
       </c>
       <c r="N65" s="71" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="P65" t="s">
         <v>414</v>
@@ -5733,7 +6066,7 @@
         <v>456</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
     </row>
     <row r="67" spans="1:16">
@@ -5772,7 +6105,7 @@
         <v>402</v>
       </c>
       <c r="N68" s="75" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="P68" t="s">
         <v>216</v>
@@ -5810,6 +6143,9 @@
         <f>SUM(D69:I69)</f>
         <v>392</v>
       </c>
+      <c r="K69" s="69" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="70" spans="1:16">
       <c r="A70" t="s">
@@ -5877,7 +6213,7 @@
         <v>400</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="P71" t="s">
         <v>260</v>
@@ -5916,7 +6252,7 @@
         <v>313</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="P72" t="s">
         <v>262</v>
@@ -6024,13 +6360,13 @@
         <v>367</v>
       </c>
       <c r="K75" s="75" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="N75" s="75" t="s">
+        <v>593</v>
+      </c>
+      <c r="O75" s="73" t="s">
         <v>596</v>
-      </c>
-      <c r="O75" s="73" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="76" spans="1:16">
@@ -6102,16 +6438,16 @@
         <v>328</v>
       </c>
       <c r="K77" s="75" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="L77" s="73" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="M77" s="74" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="N77" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="P77" t="s">
         <v>304</v>
@@ -6153,16 +6489,16 @@
         <v>425</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="M78" s="70" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="N78" s="74" t="s">
+        <v>522</v>
+      </c>
+      <c r="O78" s="70" t="s">
         <v>524</v>
-      </c>
-      <c r="O78" s="70" t="s">
-        <v>526</v>
       </c>
       <c r="P78" t="s">
         <v>305</v>
@@ -6201,13 +6537,13 @@
         <v>519</v>
       </c>
       <c r="K79" s="73" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="L79" s="76" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="M79" s="75" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="P79" t="s">
         <v>303</v>
@@ -6246,7 +6582,7 @@
         <v>429</v>
       </c>
       <c r="K80" s="75" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="P80" t="s">
         <v>319</v>
@@ -6284,6 +6620,9 @@
         <f t="shared" si="4"/>
         <v>428</v>
       </c>
+      <c r="O81" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="83" spans="1:16">
       <c r="A83" t="s">
@@ -6317,8 +6656,11 @@
         <f t="shared" ref="J83:J92" si="5">SUM(D83:I83)</f>
         <v>351</v>
       </c>
+      <c r="L83" s="69" t="s">
+        <v>555</v>
+      </c>
       <c r="O83" s="73" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="84" spans="1:16">
@@ -6354,10 +6696,10 @@
         <v>379</v>
       </c>
       <c r="K84" s="74" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="N84" s="74" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="85" spans="1:16">
@@ -6393,13 +6735,13 @@
         <v>367</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="N85" s="73" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="O85" s="74" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="86" spans="1:16">
@@ -6435,13 +6777,16 @@
         <v>401</v>
       </c>
       <c r="L86" s="74" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="M86" s="73" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="N86" s="74" t="s">
-        <v>536</v>
+        <v>534</v>
+      </c>
+      <c r="O86" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="87" spans="1:16">
@@ -6477,10 +6822,10 @@
         <v>412</v>
       </c>
       <c r="K87" s="73" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="N87" s="74" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="88" spans="1:16">
@@ -6516,7 +6861,7 @@
         <v>381</v>
       </c>
       <c r="L88" s="75" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="89" spans="1:16">
@@ -6552,7 +6897,7 @@
         <v>395</v>
       </c>
       <c r="L89" s="75" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="90" spans="1:16">
@@ -6624,10 +6969,10 @@
         <v>387</v>
       </c>
       <c r="L91" s="73" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="O91" s="73" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="92" spans="1:16">
@@ -6663,7 +7008,10 @@
         <v>392</v>
       </c>
       <c r="L92" s="74" t="s">
-        <v>515</v>
+        <v>513</v>
+      </c>
+      <c r="N92" s="74" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="94" spans="1:16">
@@ -6699,10 +7047,10 @@
         <v>318</v>
       </c>
       <c r="N94" s="73" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="O94" s="70" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="95" spans="1:16">
@@ -6737,6 +7085,15 @@
         <f t="shared" si="6"/>
         <v>402</v>
       </c>
+      <c r="K95" s="74" t="s">
+        <v>642</v>
+      </c>
+      <c r="L95" s="75" t="s">
+        <v>527</v>
+      </c>
+      <c r="N95" s="74" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="96" spans="1:16">
       <c r="A96" t="s">
@@ -6771,19 +7128,19 @@
         <v>415</v>
       </c>
       <c r="K96" s="75" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="L96" s="4" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="M96" s="73" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N96" s="70" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="O96" s="69" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="P96" t="s">
         <v>314</v>
@@ -6822,19 +7179,19 @@
         <v>435</v>
       </c>
       <c r="K97" s="75" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="L97" s="4" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="M97" s="73" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N97" s="75" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="O97" s="69" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="P97" t="s">
         <v>315</v>
@@ -6873,19 +7230,19 @@
         <v>435</v>
       </c>
       <c r="K98" s="75" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="L98" s="4" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="M98" s="73" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N98" s="72" t="s">
         <v>435</v>
       </c>
       <c r="O98" s="69" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="P98" t="s">
         <v>316</v>
@@ -6923,6 +7280,9 @@
         <f t="shared" si="6"/>
         <v>396</v>
       </c>
+      <c r="L99" s="75" t="s">
+        <v>527</v>
+      </c>
       <c r="P99" t="s">
         <v>310</v>
       </c>
@@ -6960,7 +7320,7 @@
         <v>431</v>
       </c>
       <c r="K100" s="69" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="101" spans="1:16">
@@ -6996,10 +7356,10 @@
         <v>640</v>
       </c>
       <c r="K101" s="75" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="M101" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="102" spans="1:16">
@@ -7035,13 +7395,13 @@
         <v>670</v>
       </c>
       <c r="K102" s="75" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="L102" s="70" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="M102" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="103" spans="1:16">
@@ -7077,7 +7437,7 @@
         <v>735</v>
       </c>
       <c r="K103" s="69" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="104" spans="1:16">
@@ -7113,10 +7473,10 @@
         <v>700</v>
       </c>
       <c r="K104" s="75" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="M104" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="105" spans="1:16">
@@ -7152,10 +7512,10 @@
         <v>700</v>
       </c>
       <c r="K105" s="75" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="M105" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="106" spans="1:16">
@@ -7191,10 +7551,10 @@
         <v>867</v>
       </c>
       <c r="K106" s="75" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="M106" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="108" spans="1:16">
@@ -7229,6 +7589,9 @@
         <f t="shared" ref="J108:J116" si="7">SUM(D108:I108)</f>
         <v>459</v>
       </c>
+      <c r="N108" s="74" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="109" spans="1:16">
       <c r="A109" t="s">
@@ -7263,13 +7626,13 @@
         <v>430</v>
       </c>
       <c r="K109" s="69" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="L109" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="M109" s="69" t="s">
         <v>487</v>
-      </c>
-      <c r="M109" s="69" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="110" spans="1:16">
@@ -7305,19 +7668,19 @@
         <v>439</v>
       </c>
       <c r="K110" s="69" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="L110" s="69" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M110" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="N110" s="72" t="s">
         <v>436</v>
       </c>
       <c r="O110" s="73" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="111" spans="1:16">
@@ -7353,10 +7716,13 @@
         <v>334</v>
       </c>
       <c r="K111" s="58" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="N111" s="71" t="s">
-        <v>511</v>
+        <v>509</v>
+      </c>
+      <c r="O111" s="4" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="112" spans="1:16">
@@ -7392,7 +7758,10 @@
         <v>444</v>
       </c>
       <c r="K112" s="58" t="s">
-        <v>451</v>
+        <v>450</v>
+      </c>
+      <c r="O112" s="4" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="113" spans="1:16">
@@ -7428,7 +7797,7 @@
         <v>501</v>
       </c>
       <c r="O113" s="71" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="114" spans="1:16">
@@ -7464,7 +7833,7 @@
         <v>446</v>
       </c>
       <c r="N114" s="70" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="P114" t="s">
         <v>4</v>
@@ -7539,7 +7908,7 @@
         <v>386</v>
       </c>
       <c r="L116" s="73" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="P116" t="s">
         <v>306</v>
@@ -7951,57 +8320,57 @@
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -8014,7 +8383,7 @@
         <v>118</v>
       </c>
       <c r="D12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -8022,7 +8391,7 @@
         <v>193</v>
       </c>
       <c r="D13" s="54" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -8050,47 +8419,47 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="B22" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="B26" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -8100,11 +8469,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L132"/>
+  <dimension ref="A1:L153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8149,9 +8518,11 @@
         <v>135</v>
       </c>
       <c r="B2" s="69" t="s">
-        <v>557</v>
-      </c>
-      <c r="C2" s="5"/>
+        <v>555</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>446</v>
+      </c>
       <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
@@ -8167,9 +8538,11 @@
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="69" t="s">
-        <v>558</v>
-      </c>
-      <c r="C3" s="5"/>
+        <v>556</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>446</v>
+      </c>
       <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
@@ -8185,16 +8558,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="B4" s="69" t="s">
-        <v>423</v>
+        <v>536</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>550</v>
+        <v>446</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="50">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F4" s="50">
         <v>2</v>
@@ -8203,104 +8576,118 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8">
       <c r="B5" s="69" t="s">
-        <v>438</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>439</v>
+        <v>423</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>548</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>447</v>
+        <v>11</v>
       </c>
       <c r="E5" s="50">
-        <v>0</v>
-      </c>
-      <c r="F5" s="50" t="s">
-        <v>448</v>
+        <v>45</v>
+      </c>
+      <c r="F5" s="50">
+        <v>2</v>
       </c>
       <c r="G5" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30">
       <c r="B6" s="69" t="s">
+        <v>438</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>439</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E6" s="50">
+        <v>0</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>447</v>
+      </c>
+      <c r="G6" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30">
+      <c r="B7" s="69" t="s">
+        <v>452</v>
+      </c>
+      <c r="C7" s="47" t="s">
         <v>453</v>
       </c>
-      <c r="C6" s="47" t="s">
-        <v>454</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E7" s="50">
         <v>110</v>
       </c>
-      <c r="F6" s="50">
+      <c r="F7" s="50">
         <v>1</v>
       </c>
-      <c r="G6" s="50">
+      <c r="G7" s="50">
         <v>2</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="B7" s="69" t="s">
+    <row r="8" spans="1:8">
+      <c r="B8" s="69" t="s">
+        <v>484</v>
+      </c>
+      <c r="C8" s="47" t="s">
         <v>485</v>
       </c>
-      <c r="C7" s="47" t="s">
-        <v>486</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E8" s="50">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30">
-      <c r="B8" s="69" t="s">
+    <row r="9" spans="1:8" ht="30">
+      <c r="B9" s="69" t="s">
+        <v>487</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E9" s="50">
         <v>25</v>
       </c>
-      <c r="F8" s="50">
+      <c r="F9" s="50">
         <v>2</v>
       </c>
-      <c r="G8" s="50">
+      <c r="G9" s="50">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" s="69" t="s">
-        <v>517</v>
-      </c>
-      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:8">
       <c r="B10" s="69" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:8">
       <c r="B11" s="69" t="s">
-        <v>538</v>
+        <v>516</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:8">
       <c r="B12" s="69" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>424</v>
@@ -8320,67 +8707,152 @@
     </row>
     <row r="13" spans="1:8">
       <c r="B13" s="69" t="s">
-        <v>553</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="30">
+        <v>677</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="50">
+        <v>85</v>
+      </c>
+      <c r="F13" s="50">
+        <v>1</v>
+      </c>
+      <c r="G13" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="B14" s="69" t="s">
-        <v>610</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>608</v>
-      </c>
-      <c r="D14" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="30">
+      <c r="B15" s="69" t="s">
+        <v>606</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="50" t="s">
-        <v>609</v>
-      </c>
-      <c r="F14" s="50">
+      <c r="E15" s="50" t="s">
+        <v>605</v>
+      </c>
+      <c r="F15" s="50">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="B15" s="69"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" s="69"/>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="B17" s="69"/>
+    <row r="16" spans="1:8" ht="30">
+      <c r="B16" s="69" t="s">
+        <v>637</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>605</v>
+      </c>
+      <c r="F16" s="50">
+        <v>1</v>
+      </c>
+      <c r="G16" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="B17" s="69" t="s">
+        <v>636</v>
+      </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:7">
-      <c r="B18" s="69"/>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="B19" s="69"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="B20" s="69"/>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:7">
+    <row r="18" spans="1:8" ht="45">
+      <c r="B18" s="69" t="s">
+        <v>661</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E18" s="50">
+        <v>0</v>
+      </c>
+      <c r="F18" s="50" t="s">
+        <v>447</v>
+      </c>
+      <c r="G18" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="B19" s="69" t="s">
+        <v>675</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E19" s="50">
+        <v>0</v>
+      </c>
+      <c r="F19" s="50" t="s">
+        <v>447</v>
+      </c>
+      <c r="G19" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30">
+      <c r="B20" s="69" t="s">
+        <v>685</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>686</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E20" s="50">
+        <v>0</v>
+      </c>
+      <c r="F20" s="50" t="s">
+        <v>447</v>
+      </c>
+      <c r="G20" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="B21" s="69"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" s="59" t="s">
         <v>118</v>
       </c>
       <c r="B22" s="70" t="s">
-        <v>522</v>
+        <v>633</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>446</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E22" s="50">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F22" s="50">
         <v>1</v>
@@ -8389,70 +8861,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23" s="59"/>
       <c r="B23" s="70" t="s">
-        <v>537</v>
+        <v>535</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>446</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="50">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F23" s="50">
         <v>2</v>
       </c>
       <c r="G23" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30">
       <c r="A24" s="59"/>
       <c r="B24" s="70" t="s">
-        <v>445</v>
+        <v>520</v>
       </c>
       <c r="C24" s="47" t="s">
-        <v>446</v>
+        <v>634</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E24" s="50">
-        <v>60</v>
-      </c>
-      <c r="F24" s="50" t="s">
-        <v>448</v>
+        <v>50</v>
+      </c>
+      <c r="F24" s="50">
+        <v>1</v>
       </c>
       <c r="G24" s="50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30">
       <c r="A25" s="59"/>
       <c r="B25" s="70" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C25" s="47" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E25" s="50">
         <v>0</v>
       </c>
       <c r="F25" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G25" s="50">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="60">
+    <row r="26" spans="1:8" ht="60">
       <c r="A26" s="59"/>
       <c r="B26" s="70" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>11</v>
@@ -8467,13 +8942,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="60">
+    <row r="27" spans="1:8" ht="60">
       <c r="A27" s="59"/>
       <c r="B27" s="70" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C27" s="47" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>0</v>
@@ -8488,218 +8963,281 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8" ht="30">
       <c r="A28" s="59"/>
-      <c r="B28" s="70"/>
-    </row>
-    <row r="29" spans="1:7" ht="30">
+      <c r="B28" s="70" t="s">
+        <v>537</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>563</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="50">
+        <v>55</v>
+      </c>
+      <c r="F28" s="50">
+        <v>2</v>
+      </c>
+      <c r="G28" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="59"/>
       <c r="B29" s="70" t="s">
         <v>539</v>
       </c>
-      <c r="C29" s="47" t="s">
-        <v>565</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" s="50">
-        <v>55</v>
-      </c>
-      <c r="F29" s="50">
-        <v>2</v>
-      </c>
-      <c r="G29" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="59"/>
       <c r="B30" s="70" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>617</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="50">
+        <v>55</v>
+      </c>
+      <c r="F30" s="50">
+        <v>1</v>
+      </c>
+      <c r="G30" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="59"/>
       <c r="B31" s="70" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30">
-      <c r="A32" s="60" t="s">
-        <v>193</v>
-      </c>
-      <c r="B32" s="71" t="s">
-        <v>425</v>
+        <v>651</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="50">
+        <v>60</v>
+      </c>
+      <c r="F31" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="G31" s="50">
+        <v>2</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="59"/>
+      <c r="B32" s="70" t="s">
+        <v>662</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>426</v>
+        <v>663</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="E32" s="50">
+        <v>50</v>
+      </c>
+      <c r="F32" s="50">
+        <v>1</v>
       </c>
       <c r="G32" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="59"/>
+      <c r="B33" s="70"/>
+    </row>
+    <row r="34" spans="1:9" ht="30">
+      <c r="A34" s="59"/>
+      <c r="B34" s="70" t="s">
+        <v>445</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>648</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E34" s="50">
+        <v>0</v>
+      </c>
+      <c r="F34" s="50" t="s">
+        <v>447</v>
+      </c>
+      <c r="G34" s="50">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="60"/>
-      <c r="B33" s="71" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="30">
-      <c r="A34" s="60"/>
-      <c r="B34" s="71" t="s">
-        <v>511</v>
-      </c>
-      <c r="C34" s="47" t="s">
-        <v>512</v>
-      </c>
-      <c r="D34" s="6" t="s">
+    <row r="35" spans="1:9" ht="30">
+      <c r="A35" s="59"/>
+      <c r="B35" s="70" t="s">
+        <v>543</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E35" s="50">
         <v>0</v>
       </c>
-      <c r="E34" s="50">
-        <v>50</v>
-      </c>
-      <c r="F34" s="50">
-        <v>1</v>
-      </c>
-      <c r="G34" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="45">
-      <c r="A35" s="60"/>
-      <c r="B35" s="71" t="s">
-        <v>513</v>
-      </c>
-      <c r="C35" s="47" t="s">
-        <v>586</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="50">
-        <v>55</v>
-      </c>
-      <c r="F35" s="50">
-        <v>1</v>
+      <c r="F35" s="50" t="s">
+        <v>447</v>
       </c>
       <c r="G35" s="50">
         <v>3</v>
       </c>
-      <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="60"/>
-      <c r="B36" s="71" t="s">
-        <v>519</v>
-      </c>
-      <c r="I36" s="17"/>
+      <c r="A36" s="59"/>
+      <c r="B36" s="70" t="s">
+        <v>644</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>646</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E36" s="50">
+        <v>0</v>
+      </c>
+      <c r="F36" s="50" t="s">
+        <v>645</v>
+      </c>
+      <c r="G36" s="50">
+        <v>2</v>
+      </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="60"/>
+      <c r="A37" s="60" t="s">
+        <v>193</v>
+      </c>
       <c r="B37" s="71" t="s">
-        <v>544</v>
-      </c>
-      <c r="I37" s="17"/>
-    </row>
-    <row r="38" spans="1:9">
+        <v>508</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="50">
+        <v>60</v>
+      </c>
+      <c r="F37" s="50">
+        <v>1</v>
+      </c>
+      <c r="G37" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30">
       <c r="A38" s="60"/>
       <c r="B38" s="71" t="s">
-        <v>552</v>
-      </c>
-      <c r="I38" s="17"/>
-    </row>
-    <row r="39" spans="1:9">
+        <v>509</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="50">
+        <v>50</v>
+      </c>
+      <c r="F38" s="50">
+        <v>1</v>
+      </c>
+      <c r="G38" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="45">
       <c r="A39" s="60"/>
       <c r="B39" s="71" t="s">
-        <v>554</v>
+        <v>511</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>584</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="50">
+        <v>55</v>
+      </c>
+      <c r="F39" s="50">
+        <v>1</v>
+      </c>
+      <c r="G39" s="50">
+        <v>3</v>
       </c>
       <c r="I39" s="17"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" ht="30">
       <c r="A40" s="60"/>
       <c r="B40" s="71" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="C40" s="47" t="s">
-        <v>486</v>
+        <v>654</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E40" s="50">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F40" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G40" s="50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="60"/>
       <c r="B41" s="71" t="s">
-        <v>617</v>
-      </c>
-      <c r="C41" s="47" t="s">
-        <v>618</v>
-      </c>
-      <c r="D41" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="I41" s="17"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="60"/>
+      <c r="B42" s="71" t="s">
+        <v>542</v>
+      </c>
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="60"/>
+      <c r="B43" s="71" t="s">
+        <v>552</v>
+      </c>
+      <c r="I43" s="17"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="60"/>
+      <c r="B44" s="71" t="s">
+        <v>583</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>485</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="50">
-        <v>100</v>
-      </c>
-      <c r="F41" s="50">
-        <v>1</v>
-      </c>
-      <c r="G41" s="50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="61" t="s">
-        <v>194</v>
-      </c>
-      <c r="B42" s="73" t="s">
-        <v>492</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="30">
-      <c r="A43" s="61"/>
-      <c r="B43" s="73" t="s">
-        <v>506</v>
-      </c>
-      <c r="C43" s="47" t="s">
-        <v>507</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" s="50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="45">
-      <c r="A44" s="61"/>
-      <c r="B44" s="73" t="s">
-        <v>514</v>
-      </c>
-      <c r="C44" s="47" t="s">
-        <v>586</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="E44" s="50">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="F44" s="50">
         <v>1</v>
@@ -8708,335 +9246,405 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="61"/>
-      <c r="B45" s="73" t="s">
-        <v>531</v>
+    <row r="45" spans="1:9" ht="45">
+      <c r="A45" s="60"/>
+      <c r="B45" s="71" t="s">
+        <v>613</v>
+      </c>
+      <c r="C45" s="47" t="s">
+        <v>614</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E45" s="50">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="F45" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G45" s="50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="60"/>
+      <c r="B46" s="71" t="s">
+        <v>550</v>
+      </c>
+      <c r="I46" s="17"/>
+    </row>
+    <row r="47" spans="1:9" ht="30">
+      <c r="A47" s="60"/>
+      <c r="B47" s="71" t="s">
+        <v>425</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E47" s="50">
+        <v>0</v>
+      </c>
+      <c r="F47" s="50" t="s">
+        <v>447</v>
+      </c>
+      <c r="G47" s="50">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="61"/>
-      <c r="B46" s="73" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="61"/>
-      <c r="B47" s="73" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="30">
-      <c r="A48" s="61"/>
+    <row r="48" spans="1:9">
+      <c r="A48" s="61" t="s">
+        <v>194</v>
+      </c>
       <c r="B48" s="73" t="s">
-        <v>594</v>
-      </c>
-      <c r="C48" s="47" t="s">
-        <v>595</v>
+        <v>491</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="50">
-        <v>60</v>
-      </c>
-      <c r="F48" s="50">
-        <v>2</v>
-      </c>
-      <c r="G48" s="50">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30">
       <c r="A49" s="61"/>
       <c r="B49" s="73" t="s">
-        <v>599</v>
+        <v>505</v>
       </c>
       <c r="C49" s="47" t="s">
-        <v>561</v>
+        <v>506</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="50">
-        <v>65</v>
-      </c>
-      <c r="F49" s="50">
+        <v>11</v>
+      </c>
+      <c r="G49" s="50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="45">
+      <c r="A50" s="61"/>
+      <c r="B50" s="73" t="s">
+        <v>512</v>
+      </c>
+      <c r="C50" s="47" t="s">
+        <v>584</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="50">
+        <v>55</v>
+      </c>
+      <c r="F50" s="50">
         <v>1</v>
       </c>
-      <c r="G49" s="50">
+      <c r="G50" s="50">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="61"/>
-      <c r="B50" s="73"/>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="61"/>
-      <c r="B51" s="73"/>
+      <c r="B51" s="73" t="s">
+        <v>529</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="50">
+        <v>70</v>
+      </c>
+      <c r="F51" s="50">
+        <v>2</v>
+      </c>
+      <c r="G51" s="50">
+        <v>3</v>
+      </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="B52" s="74" t="s">
-        <v>515</v>
-      </c>
-      <c r="C52" s="47" t="s">
-        <v>562</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="50">
-        <v>65</v>
-      </c>
-      <c r="F52" s="50">
-        <v>2</v>
-      </c>
-      <c r="G52" s="50">
-        <v>2</v>
+      <c r="A52" s="61"/>
+      <c r="B52" s="73" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="62"/>
-      <c r="B53" s="74" t="s">
-        <v>524</v>
-      </c>
-      <c r="C53" s="47" t="s">
-        <v>607</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="50">
-        <v>45</v>
-      </c>
-      <c r="F53" s="50">
-        <v>1</v>
-      </c>
-      <c r="G53" s="50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="62"/>
-      <c r="B54" s="74" t="s">
-        <v>536</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>563</v>
+      <c r="A53" s="61"/>
+      <c r="B53" s="73" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="30">
+      <c r="A54" s="61"/>
+      <c r="B54" s="73" t="s">
+        <v>591</v>
+      </c>
+      <c r="C54" s="47" t="s">
+        <v>592</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E54" s="50">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F54" s="50">
         <v>2</v>
       </c>
       <c r="G54" s="50">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30">
-      <c r="A55" s="62"/>
-      <c r="B55" s="74" t="s">
-        <v>560</v>
+      <c r="A55" s="61"/>
+      <c r="B55" s="73" t="s">
+        <v>596</v>
       </c>
       <c r="C55" s="47" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E55" s="50">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F55" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G55" s="50">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="45">
-      <c r="A56" s="62"/>
-      <c r="B56" s="74" t="s">
-        <v>573</v>
-      </c>
-      <c r="C56" s="47" t="s">
-        <v>574</v>
-      </c>
-      <c r="D56" s="6" t="s">
+    <row r="56" spans="1:7">
+      <c r="A56" s="61"/>
+      <c r="B56" s="73" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="61"/>
+      <c r="B57" s="73" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="45">
+      <c r="A58" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B58" s="74" t="s">
+        <v>513</v>
+      </c>
+      <c r="C58" s="47" t="s">
+        <v>635</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E56" s="50">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="45">
-      <c r="A57" s="62"/>
-      <c r="B57" s="74" t="s">
-        <v>612</v>
-      </c>
-      <c r="C57" s="47" t="s">
-        <v>574</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="50">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="62"/>
-      <c r="B58" s="74"/>
+      <c r="E58" s="50">
+        <v>60</v>
+      </c>
+      <c r="F58" s="50">
+        <v>2</v>
+      </c>
+      <c r="G58" s="50">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="62"/>
-      <c r="B59" s="74"/>
+      <c r="B59" s="74" t="s">
+        <v>522</v>
+      </c>
+      <c r="C59" s="47" t="s">
+        <v>603</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="50">
+        <v>45</v>
+      </c>
+      <c r="F59" s="50">
+        <v>1</v>
+      </c>
+      <c r="G59" s="50">
+        <v>3</v>
+      </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="62"/>
-      <c r="B60" s="74"/>
+      <c r="B60" s="74" t="s">
+        <v>534</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="50">
+        <v>50</v>
+      </c>
+      <c r="F60" s="50">
+        <v>2</v>
+      </c>
+      <c r="G60" s="50">
+        <v>3</v>
+      </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="62"/>
-      <c r="B61" s="74"/>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="63" t="s">
-        <v>191</v>
-      </c>
-      <c r="B62" s="75" t="s">
-        <v>498</v>
+      <c r="B61" s="74" t="s">
+        <v>687</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>688</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="50">
+        <v>45</v>
+      </c>
+      <c r="F61" s="50">
+        <v>2</v>
+      </c>
+      <c r="G61" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30">
+      <c r="A62" s="62"/>
+      <c r="B62" s="74" t="s">
+        <v>558</v>
+      </c>
+      <c r="C62" s="47" t="s">
+        <v>559</v>
       </c>
       <c r="D62" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="50">
+        <v>55</v>
+      </c>
+      <c r="F62" s="50">
+        <v>2</v>
+      </c>
+      <c r="G62" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="45">
+      <c r="A63" s="62"/>
+      <c r="B63" s="74" t="s">
+        <v>571</v>
+      </c>
+      <c r="C63" s="47" t="s">
+        <v>572</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="50">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="45">
+      <c r="A64" s="62"/>
+      <c r="B64" s="74" t="s">
+        <v>608</v>
+      </c>
+      <c r="C64" s="47" t="s">
+        <v>572</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="63"/>
-      <c r="B63" s="75" t="s">
-        <v>564</v>
-      </c>
-      <c r="C63" s="47" t="s">
-        <v>562</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63" s="50">
+      <c r="E64" s="50">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="45">
+      <c r="A65" s="62"/>
+      <c r="B65" s="74" t="s">
+        <v>642</v>
+      </c>
+      <c r="C65" s="47" t="s">
+        <v>643</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="50">
         <v>70</v>
       </c>
-      <c r="F63" s="50">
+      <c r="F65" s="50">
         <v>1</v>
       </c>
-      <c r="G63" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="63"/>
-      <c r="B64" s="75" t="s">
-        <v>500</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="50">
-        <v>80</v>
-      </c>
-      <c r="F64" s="50">
-        <v>2</v>
-      </c>
-      <c r="G64" s="50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="63"/>
-      <c r="B65" s="75" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="63"/>
-      <c r="B66" s="75" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="30">
-      <c r="A67" s="63"/>
-      <c r="B67" s="75" t="s">
-        <v>582</v>
+      <c r="G65" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="62"/>
+      <c r="B66" s="74" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30">
+      <c r="A67" s="62"/>
+      <c r="B67" s="74" t="s">
+        <v>690</v>
       </c>
       <c r="C67" s="47" t="s">
-        <v>598</v>
+        <v>691</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="50">
+        <v>50</v>
+      </c>
+      <c r="F67" s="50">
+        <v>2</v>
+      </c>
+      <c r="G67" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="30">
+      <c r="A68" s="62"/>
+      <c r="B68" s="74" t="s">
+        <v>649</v>
+      </c>
+      <c r="C68" s="47" t="s">
+        <v>650</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E68" s="50">
         <v>0</v>
       </c>
-      <c r="F67" s="50" t="s">
-        <v>589</v>
-      </c>
-      <c r="G67" s="50">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="45">
-      <c r="A68" s="63"/>
-      <c r="B68" s="75" t="s">
-        <v>596</v>
-      </c>
-      <c r="C68" s="47" t="s">
-        <v>597</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="50">
-        <v>50</v>
-      </c>
-      <c r="F68" s="50">
-        <v>2</v>
+      <c r="F68" s="50" t="s">
+        <v>447</v>
       </c>
       <c r="G68" s="50">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="63"/>
-      <c r="B69" s="75" t="s">
-        <v>602</v>
+    <row r="69" spans="1:7" ht="30">
+      <c r="A69" s="62"/>
+      <c r="B69" s="74" t="s">
+        <v>673</v>
       </c>
       <c r="C69" s="47" t="s">
-        <v>486</v>
+        <v>674</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>11</v>
+        <v>446</v>
       </c>
       <c r="E69" s="50">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F69" s="50">
         <v>2</v>
@@ -9045,578 +9653,966 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="63"/>
-      <c r="B70" s="75"/>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="63"/>
-      <c r="B71" s="75"/>
-    </row>
-    <row r="72" spans="1:8" ht="30">
-      <c r="A72" s="64" t="s">
+    <row r="70" spans="1:7" ht="30">
+      <c r="A70" s="62"/>
+      <c r="B70" s="74" t="s">
+        <v>670</v>
+      </c>
+      <c r="C70" s="47" t="s">
+        <v>671</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E70" s="50">
+        <v>0</v>
+      </c>
+      <c r="F70" s="50" t="s">
+        <v>586</v>
+      </c>
+      <c r="G70" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="30">
+      <c r="A71" s="62"/>
+      <c r="B71" s="74" t="s">
+        <v>680</v>
+      </c>
+      <c r="C71" s="47" t="s">
+        <v>681</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E71" s="50">
+        <v>0</v>
+      </c>
+      <c r="F71" s="50" t="s">
+        <v>447</v>
+      </c>
+      <c r="G71" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="62"/>
+      <c r="B72" s="74" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B73" s="75" t="s">
+        <v>497</v>
+      </c>
+      <c r="C73" s="47" t="s">
+        <v>446</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="50">
+        <v>70</v>
+      </c>
+      <c r="F73" s="50">
+        <v>1</v>
+      </c>
+      <c r="G73" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="63"/>
+      <c r="B74" s="75" t="s">
+        <v>499</v>
+      </c>
+      <c r="C74" s="47" t="s">
+        <v>446</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" s="50">
+        <v>80</v>
+      </c>
+      <c r="F74" s="50">
+        <v>2</v>
+      </c>
+      <c r="G74" s="50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="63"/>
+      <c r="B75" s="75" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="63"/>
+      <c r="B76" s="75" t="s">
+        <v>562</v>
+      </c>
+      <c r="C76" s="47" t="s">
+        <v>560</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="50">
+        <v>70</v>
+      </c>
+      <c r="F76" s="50">
+        <v>1</v>
+      </c>
+      <c r="G76" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="63"/>
+      <c r="B77" s="75" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="63"/>
+      <c r="B78" s="75" t="s">
+        <v>527</v>
+      </c>
+      <c r="C78" s="47" t="s">
+        <v>621</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="50">
+        <v>40</v>
+      </c>
+      <c r="F78" s="50">
+        <v>2</v>
+      </c>
+      <c r="G78" s="50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="30">
+      <c r="A79" s="63"/>
+      <c r="B79" s="75" t="s">
+        <v>580</v>
+      </c>
+      <c r="C79" s="47" t="s">
+        <v>595</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="50">
+        <v>0</v>
+      </c>
+      <c r="F79" s="50" t="s">
+        <v>586</v>
+      </c>
+      <c r="G79" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="45">
+      <c r="A80" s="63"/>
+      <c r="B80" s="75" t="s">
+        <v>593</v>
+      </c>
+      <c r="C80" s="47" t="s">
+        <v>594</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="50">
+        <v>50</v>
+      </c>
+      <c r="F80" s="50">
+        <v>2</v>
+      </c>
+      <c r="G80" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="63"/>
+      <c r="B81" s="75" t="s">
+        <v>599</v>
+      </c>
+      <c r="C81" s="47" t="s">
+        <v>485</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="50">
+        <v>50</v>
+      </c>
+      <c r="F81" s="50">
+        <v>2</v>
+      </c>
+      <c r="G81" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="30">
+      <c r="A82" s="63"/>
+      <c r="B82" s="75" t="s">
+        <v>665</v>
+      </c>
+      <c r="C82" s="47" t="s">
+        <v>666</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="50">
+        <v>100</v>
+      </c>
+      <c r="F82" s="50">
+        <v>2</v>
+      </c>
+      <c r="G82" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="63"/>
+      <c r="B83" s="75"/>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="B72" s="72" t="s">
+      <c r="B84" s="72" t="s">
+        <v>521</v>
+      </c>
+      <c r="C84" s="47" t="s">
+        <v>446</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="50">
+        <v>60</v>
+      </c>
+      <c r="F84" s="50">
+        <v>2</v>
+      </c>
+      <c r="G84" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="64"/>
+      <c r="B85" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="C85" s="47" t="s">
+        <v>660</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" s="50">
+        <v>50</v>
+      </c>
+      <c r="F85" s="50" t="s">
+        <v>605</v>
+      </c>
+      <c r="G85" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="64"/>
+      <c r="B86" s="72" t="s">
+        <v>523</v>
+      </c>
+      <c r="C86" s="47" t="s">
+        <v>657</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" s="50">
+        <v>50</v>
+      </c>
+      <c r="F86" s="50">
+        <v>1</v>
+      </c>
+      <c r="G86" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="30">
+      <c r="A87" s="64"/>
+      <c r="B87" s="72" t="s">
+        <v>435</v>
+      </c>
+      <c r="C87" s="47" t="s">
+        <v>489</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" s="50">
+        <v>50</v>
+      </c>
+      <c r="F87" s="50">
+        <v>2</v>
+      </c>
+      <c r="G87" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="64"/>
+      <c r="B88" s="72" t="s">
+        <v>622</v>
+      </c>
+      <c r="C88" s="47" t="s">
+        <v>621</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="50">
+        <v>70</v>
+      </c>
+      <c r="F88" s="50">
+        <v>2</v>
+      </c>
+      <c r="G88" s="50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="30">
+      <c r="A89" s="64"/>
+      <c r="B89" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="C89" s="47" t="s">
+        <v>507</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89" s="50">
+        <v>75</v>
+      </c>
+      <c r="F89" s="50" t="s">
+        <v>605</v>
+      </c>
+      <c r="G89" s="50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="64"/>
+      <c r="B90" s="72" t="s">
+        <v>538</v>
+      </c>
+      <c r="C90" s="47" t="s">
+        <v>446</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E90" s="50">
+        <v>70</v>
+      </c>
+      <c r="F90" s="50">
+        <v>2</v>
+      </c>
+      <c r="G90" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="45">
+      <c r="A91" s="64"/>
+      <c r="B91" s="72" t="s">
+        <v>585</v>
+      </c>
+      <c r="C91" s="47" t="s">
+        <v>630</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="50">
+        <v>50</v>
+      </c>
+      <c r="F91" s="50" t="s">
+        <v>586</v>
+      </c>
+      <c r="G91" s="50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="45">
+      <c r="A92" s="64"/>
+      <c r="B92" s="72" t="s">
+        <v>631</v>
+      </c>
+      <c r="C92" s="47" t="s">
+        <v>656</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="50">
+        <v>80</v>
+      </c>
+      <c r="F92" s="50">
+        <v>1</v>
+      </c>
+      <c r="G92" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="30">
+      <c r="A93" s="64"/>
+      <c r="B93" s="72" t="s">
         <v>436</v>
       </c>
-      <c r="C72" s="47" t="s">
+      <c r="C93" s="47" t="s">
         <v>437</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="D93" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E93" s="50">
+        <v>0</v>
+      </c>
+      <c r="F93" s="50" t="s">
         <v>447</v>
       </c>
-      <c r="E72" s="50">
+      <c r="G93" s="50">
+        <v>2</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="64"/>
+      <c r="B94" s="72" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99" s="51" t="s">
+        <v>440</v>
+      </c>
+      <c r="L99" s="56"/>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="C100" s="47" t="s">
+        <v>490</v>
+      </c>
+      <c r="L100" s="56"/>
+    </row>
+    <row r="101" spans="1:12" ht="30">
+      <c r="B101" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="C101" s="47" t="s">
+        <v>575</v>
+      </c>
+      <c r="L101" s="56"/>
+    </row>
+    <row r="102" spans="1:12">
+      <c r="B102" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="L102" s="56"/>
+    </row>
+    <row r="103" spans="1:12">
+      <c r="B103" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="L103" s="56"/>
+    </row>
+    <row r="104" spans="1:12" ht="30">
+      <c r="B104" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="C104" s="47" t="s">
+        <v>574</v>
+      </c>
+      <c r="L104" s="56"/>
+    </row>
+    <row r="105" spans="1:12" ht="60">
+      <c r="B105" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C105" s="47" t="s">
+        <v>578</v>
+      </c>
+      <c r="L105" s="56"/>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="B106" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="L106" s="56"/>
+    </row>
+    <row r="107" spans="1:12" ht="30">
+      <c r="B107" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="C107" s="47" t="s">
+        <v>582</v>
+      </c>
+      <c r="L107" s="56"/>
+    </row>
+    <row r="108" spans="1:12" ht="30">
+      <c r="B108" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="C108" s="47" t="s">
+        <v>639</v>
+      </c>
+      <c r="L108" s="56"/>
+    </row>
+    <row r="109" spans="1:12" ht="30">
+      <c r="B109" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="C109" s="47" t="s">
+        <v>602</v>
+      </c>
+      <c r="L109" s="56"/>
+    </row>
+    <row r="110" spans="1:12" ht="30">
+      <c r="B110" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="C110" s="47" t="s">
+        <v>611</v>
+      </c>
+      <c r="L110" s="56"/>
+    </row>
+    <row r="111" spans="1:12" ht="60">
+      <c r="B111" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="C111" s="47" t="s">
+        <v>612</v>
+      </c>
+      <c r="L111" s="56"/>
+    </row>
+    <row r="112" spans="1:12" ht="75">
+      <c r="B112" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C112" s="47" t="s">
+        <v>616</v>
+      </c>
+      <c r="L112" s="56"/>
+    </row>
+    <row r="113" spans="1:12">
+      <c r="B113" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="L113" s="56"/>
+    </row>
+    <row r="114" spans="1:12" ht="45">
+      <c r="B114" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="C114" s="47" t="s">
+        <v>629</v>
+      </c>
+      <c r="L114" s="56"/>
+    </row>
+    <row r="115" spans="1:12" ht="30">
+      <c r="B115" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="C115" s="47" t="s">
+        <v>669</v>
+      </c>
+      <c r="L115" s="56"/>
+    </row>
+    <row r="116" spans="1:12">
+      <c r="B116" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="C116" s="47" t="s">
+        <v>684</v>
+      </c>
+      <c r="L116" s="56"/>
+    </row>
+    <row r="117" spans="1:12" ht="45">
+      <c r="A117" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B117" s="57" t="s">
+        <v>532</v>
+      </c>
+      <c r="C117" s="47" t="s">
+        <v>632</v>
+      </c>
+      <c r="L117" s="56"/>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="A118" s="59"/>
+      <c r="B118" s="57"/>
+      <c r="L118" s="56"/>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="A119" s="59"/>
+      <c r="B119" s="57" t="s">
+        <v>540</v>
+      </c>
+      <c r="L119" s="56"/>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120" s="59"/>
+      <c r="B120" s="57" t="s">
+        <v>557</v>
+      </c>
+      <c r="L120" s="56"/>
+    </row>
+    <row r="121" spans="1:12" ht="30">
+      <c r="A121" s="60" t="s">
+        <v>193</v>
+      </c>
+      <c r="B121" s="58" t="s">
+        <v>450</v>
+      </c>
+      <c r="C121" s="47" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="B122" s="65"/>
+      <c r="L122" s="56"/>
+    </row>
+    <row r="123" spans="1:12" ht="45">
+      <c r="A123" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B123" s="66" t="s">
+        <v>514</v>
+      </c>
+      <c r="C123" s="47" t="s">
+        <v>655</v>
+      </c>
+      <c r="L123" s="56"/>
+    </row>
+    <row r="124" spans="1:12">
+      <c r="A124" s="62"/>
+      <c r="B124" s="66" t="s">
+        <v>541</v>
+      </c>
+      <c r="L124" s="56"/>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="A125" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B125" s="67" t="s">
+        <v>528</v>
+      </c>
+      <c r="L125" s="56"/>
+    </row>
+    <row r="126" spans="1:12">
+      <c r="A126" s="63"/>
+      <c r="B126" s="67" t="s">
+        <v>530</v>
+      </c>
+      <c r="L126" s="56"/>
+    </row>
+    <row r="127" spans="1:12" ht="30">
+      <c r="A127" s="63"/>
+      <c r="B127" s="67" t="s">
+        <v>597</v>
+      </c>
+      <c r="C127" s="47" t="s">
+        <v>598</v>
+      </c>
+      <c r="L127" s="56"/>
+    </row>
+    <row r="128" spans="1:12" ht="30">
+      <c r="A128" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B128" s="68" t="s">
+        <v>448</v>
+      </c>
+      <c r="C128" s="47" t="s">
+        <v>449</v>
+      </c>
+      <c r="H128" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L128" s="56"/>
+    </row>
+    <row r="129" spans="1:12">
+      <c r="A129" s="64"/>
+      <c r="B129" s="68" t="s">
+        <v>526</v>
+      </c>
+      <c r="L129" s="56"/>
+    </row>
+    <row r="130" spans="1:12">
+      <c r="A130" s="64"/>
+      <c r="B130" s="68" t="s">
+        <v>531</v>
+      </c>
+      <c r="L130" s="56"/>
+    </row>
+    <row r="131" spans="1:12">
+      <c r="A131" s="64"/>
+      <c r="B131" s="68" t="s">
+        <v>544</v>
+      </c>
+      <c r="L131" s="56"/>
+    </row>
+    <row r="133" spans="1:12">
+      <c r="A133" s="51" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
+      <c r="A134" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C134" s="47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
+      <c r="B135" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="C135" s="47" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
+      <c r="B136" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="C136" s="47" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
+      <c r="B137" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="C137" s="47" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
+      <c r="B138" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C138" s="47" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
+      <c r="B139" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="C139" s="47" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
+      <c r="B140" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="C140" s="47" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
+      <c r="B141" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="C141" s="47" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
+      <c r="B142" s="4" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" ht="30">
+      <c r="B143" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="C143" s="47" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" ht="45">
+      <c r="B144" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="C144" s="47" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="B145" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="C145" s="47" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B146" s="70" t="s">
+        <v>495</v>
+      </c>
+      <c r="D146" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F72" s="50" t="s">
-        <v>448</v>
-      </c>
-      <c r="G72" s="50">
-        <v>2</v>
-      </c>
-      <c r="H72" s="4" t="s">
+      <c r="E146" s="50">
+        <v>135</v>
+      </c>
+      <c r="G146" s="50">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="64"/>
-      <c r="B73" s="72" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="64"/>
-      <c r="B74" s="72" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="30">
-      <c r="A75" s="64"/>
-      <c r="B75" s="72" t="s">
-        <v>435</v>
-      </c>
-      <c r="C75" s="47" t="s">
-        <v>490</v>
-      </c>
-      <c r="D75" s="6" t="s">
+    <row r="147" spans="1:7" ht="90">
+      <c r="A147" s="59"/>
+      <c r="B147" s="70" t="s">
+        <v>566</v>
+      </c>
+      <c r="C147" s="47" t="s">
+        <v>565</v>
+      </c>
+      <c r="D147" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E75" s="50">
-        <v>45</v>
-      </c>
-      <c r="F75" s="50">
-        <v>2</v>
-      </c>
-      <c r="G75" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="30">
-      <c r="A76" s="64"/>
-      <c r="B76" s="72" t="s">
-        <v>508</v>
-      </c>
-      <c r="C76" s="47" t="s">
-        <v>509</v>
-      </c>
-      <c r="D76" s="6" t="s">
+      <c r="E147" s="50">
+        <v>25</v>
+      </c>
+      <c r="G147" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="30">
+      <c r="A148" s="60" t="s">
+        <v>193</v>
+      </c>
+      <c r="B148" s="69" t="s">
+        <v>494</v>
+      </c>
+      <c r="C148" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="D148" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E76" s="50">
-        <v>80</v>
-      </c>
-      <c r="G76" s="50">
+      <c r="E148" s="50">
+        <v>120</v>
+      </c>
+      <c r="G148" s="50">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
-      <c r="A77" s="64"/>
-      <c r="B77" s="72"/>
-    </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="64"/>
-      <c r="B78" s="72" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="45">
-      <c r="A79" s="64"/>
-      <c r="B79" s="72" t="s">
-        <v>587</v>
-      </c>
-      <c r="C79" s="47" t="s">
-        <v>588</v>
-      </c>
-      <c r="D79" s="6" t="s">
+    <row r="149" spans="1:7">
+      <c r="A149" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="B149" s="69" t="s">
+        <v>496</v>
+      </c>
+      <c r="D149" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E79" s="50">
-        <v>50</v>
-      </c>
-      <c r="F79" s="50" t="s">
+      <c r="E149" s="50">
+        <v>140</v>
+      </c>
+      <c r="G149" s="50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" s="62"/>
+      <c r="B150" s="69" t="s">
         <v>589</v>
       </c>
-      <c r="G79" s="50">
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B151" s="69" t="s">
+        <v>493</v>
+      </c>
+      <c r="D151" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E151" s="50">
+        <v>135</v>
+      </c>
+      <c r="G151" s="50">
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="64"/>
-      <c r="B80" s="72"/>
-    </row>
-    <row r="81" spans="1:12">
-      <c r="A81" s="64"/>
-      <c r="B81" s="72"/>
-    </row>
-    <row r="86" spans="1:12">
-      <c r="A86" s="51" t="s">
-        <v>440</v>
-      </c>
-      <c r="L86" s="56"/>
-    </row>
-    <row r="87" spans="1:12">
-      <c r="A87" s="4" t="s">
+    <row r="152" spans="1:7">
+      <c r="A152" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B152" s="69" t="s">
+        <v>492</v>
+      </c>
+      <c r="D152" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E152" s="50">
+        <v>140</v>
+      </c>
+      <c r="G152" s="50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B153" s="69"/>
+      <c r="D153" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E153" s="50">
         <v>135</v>
       </c>
-      <c r="B87" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="C87" s="47" t="s">
-        <v>491</v>
-      </c>
-      <c r="L87" s="56"/>
-    </row>
-    <row r="88" spans="1:12" ht="30">
-      <c r="A88" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="C88" s="47" t="s">
-        <v>577</v>
-      </c>
-      <c r="L88" s="56"/>
-    </row>
-    <row r="89" spans="1:12">
-      <c r="B89" s="4" t="s">
-        <v>520</v>
-      </c>
-      <c r="L89" s="56"/>
-    </row>
-    <row r="90" spans="1:12">
-      <c r="B90" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="L90" s="56"/>
-    </row>
-    <row r="91" spans="1:12" ht="30">
-      <c r="B91" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="C91" s="47" t="s">
-        <v>576</v>
-      </c>
-      <c r="L91" s="56"/>
-    </row>
-    <row r="92" spans="1:12" ht="60">
-      <c r="B92" s="4" t="s">
-        <v>578</v>
-      </c>
-      <c r="C92" s="47" t="s">
-        <v>580</v>
-      </c>
-      <c r="L92" s="56"/>
-    </row>
-    <row r="93" spans="1:12">
-      <c r="B93" s="4" t="s">
-        <v>579</v>
-      </c>
-      <c r="L93" s="56"/>
-    </row>
-    <row r="94" spans="1:12" ht="30">
-      <c r="B94" s="4" t="s">
-        <v>583</v>
-      </c>
-      <c r="C94" s="47" t="s">
-        <v>584</v>
-      </c>
-      <c r="L94" s="56"/>
-    </row>
-    <row r="95" spans="1:12" ht="30">
-      <c r="B95" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="C95" s="47" t="s">
-        <v>604</v>
-      </c>
-      <c r="L95" s="56"/>
-    </row>
-    <row r="96" spans="1:12" ht="30">
-      <c r="B96" s="4" t="s">
-        <v>605</v>
-      </c>
-      <c r="C96" s="47" t="s">
-        <v>606</v>
-      </c>
-      <c r="L96" s="56"/>
-    </row>
-    <row r="97" spans="1:12" ht="30">
-      <c r="B97" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="C97" s="47" t="s">
-        <v>615</v>
-      </c>
-      <c r="L97" s="56"/>
-    </row>
-    <row r="98" spans="1:12" ht="60">
-      <c r="B98" s="4" t="s">
-        <v>614</v>
-      </c>
-      <c r="C98" s="47" t="s">
-        <v>616</v>
-      </c>
-      <c r="L98" s="56"/>
-    </row>
-    <row r="99" spans="1:12">
-      <c r="A99" s="59" t="s">
-        <v>118</v>
-      </c>
-      <c r="B99" s="57" t="s">
-        <v>534</v>
-      </c>
-      <c r="L99" s="56"/>
-    </row>
-    <row r="100" spans="1:12">
-      <c r="A100" s="59"/>
-      <c r="B100" s="57"/>
-      <c r="L100" s="56"/>
-    </row>
-    <row r="101" spans="1:12">
-      <c r="A101" s="59"/>
-      <c r="B101" s="57" t="s">
-        <v>542</v>
-      </c>
-      <c r="L101" s="56"/>
-    </row>
-    <row r="102" spans="1:12">
-      <c r="A102" s="59"/>
-      <c r="B102" s="57" t="s">
-        <v>559</v>
-      </c>
-      <c r="L102" s="56"/>
-    </row>
-    <row r="103" spans="1:12" ht="30">
-      <c r="A103" s="60" t="s">
-        <v>193</v>
-      </c>
-      <c r="B103" s="58" t="s">
-        <v>451</v>
-      </c>
-      <c r="C103" s="47" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12">
-      <c r="A104" s="61" t="s">
-        <v>194</v>
-      </c>
-      <c r="B104" s="65"/>
-      <c r="L104" s="56"/>
-    </row>
-    <row r="105" spans="1:12">
-      <c r="A105" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="B105" s="66" t="s">
-        <v>516</v>
-      </c>
-      <c r="L105" s="56"/>
-    </row>
-    <row r="106" spans="1:12">
-      <c r="A106" s="62"/>
-      <c r="B106" s="66" t="s">
-        <v>543</v>
-      </c>
-      <c r="L106" s="56"/>
-    </row>
-    <row r="107" spans="1:12">
-      <c r="A107" s="63" t="s">
-        <v>191</v>
-      </c>
-      <c r="B107" s="67" t="s">
-        <v>530</v>
-      </c>
-      <c r="L107" s="56"/>
-    </row>
-    <row r="108" spans="1:12">
-      <c r="A108" s="63"/>
-      <c r="B108" s="67" t="s">
-        <v>532</v>
-      </c>
-      <c r="L108" s="56"/>
-    </row>
-    <row r="109" spans="1:12" ht="30">
-      <c r="A109" s="63"/>
-      <c r="B109" s="67" t="s">
-        <v>600</v>
-      </c>
-      <c r="C109" s="47" t="s">
-        <v>601</v>
-      </c>
-      <c r="L109" s="56"/>
-    </row>
-    <row r="110" spans="1:12" ht="30">
-      <c r="A110" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="B110" s="68" t="s">
-        <v>449</v>
-      </c>
-      <c r="C110" s="47" t="s">
-        <v>450</v>
-      </c>
-      <c r="H110" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L110" s="56"/>
-    </row>
-    <row r="111" spans="1:12">
-      <c r="A111" s="64"/>
-      <c r="B111" s="68" t="s">
-        <v>528</v>
-      </c>
-      <c r="L111" s="56"/>
-    </row>
-    <row r="112" spans="1:12">
-      <c r="A112" s="64"/>
-      <c r="B112" s="68" t="s">
-        <v>533</v>
-      </c>
-      <c r="L112" s="56"/>
-    </row>
-    <row r="113" spans="1:12">
-      <c r="A113" s="64"/>
-      <c r="B113" s="68" t="s">
-        <v>546</v>
-      </c>
-      <c r="L113" s="56"/>
-    </row>
-    <row r="115" spans="1:12">
-      <c r="A115" s="51" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12">
-      <c r="A116" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="C116" s="47" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12">
-      <c r="A117" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="C117" s="47" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12">
-      <c r="A118" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="C118" s="47" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12">
-      <c r="A119" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>460</v>
-      </c>
-      <c r="C119" s="47" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12">
-      <c r="A120" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="C120" s="47" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12">
-      <c r="A121" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>462</v>
-      </c>
-      <c r="C121" s="47" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12">
-      <c r="B122" s="4" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" ht="30">
-      <c r="B123" s="4" t="s">
-        <v>590</v>
-      </c>
-      <c r="C123" s="47" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12">
-      <c r="B124" s="4" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12">
-      <c r="A125" s="59" t="s">
-        <v>118</v>
-      </c>
-      <c r="B125" s="70" t="s">
-        <v>496</v>
-      </c>
-      <c r="D125" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E125" s="50">
-        <v>135</v>
-      </c>
-      <c r="G125" s="50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" ht="90">
-      <c r="A126" s="59"/>
-      <c r="B126" s="70" t="s">
-        <v>568</v>
-      </c>
-      <c r="C126" s="47" t="s">
-        <v>567</v>
-      </c>
-      <c r="D126" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E126" s="50">
-        <v>25</v>
-      </c>
-      <c r="G126" s="50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:12" ht="30">
-      <c r="A127" s="60" t="s">
-        <v>193</v>
-      </c>
-      <c r="B127" s="69" t="s">
-        <v>495</v>
-      </c>
-      <c r="C127" s="47" t="s">
-        <v>426</v>
-      </c>
-      <c r="D127" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E127" s="50">
-        <v>120</v>
-      </c>
-      <c r="G127" s="50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12">
-      <c r="A128" s="61" t="s">
-        <v>194</v>
-      </c>
-      <c r="B128" s="69" t="s">
-        <v>497</v>
-      </c>
-      <c r="D128" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E128" s="50">
-        <v>140</v>
-      </c>
-      <c r="G128" s="50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7">
-      <c r="A129" s="62"/>
-      <c r="B129" s="69" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7">
-      <c r="A130" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="B130" s="69" t="s">
-        <v>494</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E130" s="50">
-        <v>135</v>
-      </c>
-      <c r="G130" s="50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7">
-      <c r="A131" s="63" t="s">
-        <v>191</v>
-      </c>
-      <c r="B131" s="69" t="s">
-        <v>493</v>
-      </c>
-      <c r="D131" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E131" s="50">
-        <v>140</v>
-      </c>
-      <c r="G131" s="50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7">
-      <c r="A132" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="B132" s="69"/>
-      <c r="D132" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E132" s="50">
-        <v>135</v>
-      </c>
-      <c r="G132" s="50">
+      <c r="G153" s="50">
         <v>4</v>
       </c>
     </row>
@@ -10646,7 +11642,7 @@
         <v>1</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C49" s="8">
         <v>1</v>
@@ -11168,10 +12164,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:A35"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11359,43 +12355,66 @@
         <v>146</v>
       </c>
     </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="17" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="17" t="s">
+        <v>640</v>
+      </c>
+    </row>
     <row r="38" spans="1:2">
       <c r="A38" s="17" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="17" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="17"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="17" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="B40" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="B41" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="B42" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="B43" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="B44" s="16" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="B45" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="B46" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="B47" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="B48" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="B49" s="16" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="B50" s="16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="16" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="16" t="s">
         <v>434</v>
       </c>
     </row>
@@ -11409,8 +12428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added more passive skills
</commit_message>
<xml_diff>
--- a/Documentation.xlsx
+++ b/Documentation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Overview" sheetId="2" r:id="rId1"/>
@@ -21,21 +21,17 @@
     <sheet name="Religions" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="899">
   <si>
     <t>physical</t>
   </si>
@@ -1717,9 +1713,6 @@
     <t>Blood Boil</t>
   </si>
   <si>
-    <t>Unit deals massively increased damage (60%) while below 50% max Health.</t>
-  </si>
-  <si>
     <t>Black Blade</t>
   </si>
   <si>
@@ -2711,6 +2704,30 @@
   </si>
   <si>
     <t>Boost element/type damage by 20%; boost magical/physical damage by 10%</t>
+  </si>
+  <si>
+    <t>Unbreaking Resolve</t>
+  </si>
+  <si>
+    <t>Volatile Flesh</t>
+  </si>
+  <si>
+    <t>At the end of every round, decrease health by 5% and inflict Poison(2) on two random enemies.</t>
+  </si>
+  <si>
+    <t>Bottomfeeder</t>
+  </si>
+  <si>
+    <t>If this ability kills enemy unit, heal self for 25% of target's max health.</t>
+  </si>
+  <si>
+    <t>Unleashed</t>
+  </si>
+  <si>
+    <t>Unit deals massively increased damage (60%) while below 50% max Health and heals for 20% of damage dealt.</t>
+  </si>
+  <si>
+    <t>When unit drops below 50% health, increases Spd/Atk by two.</t>
   </si>
 </sst>
 </file>
@@ -4564,7 +4581,7 @@
         <v>208</v>
       </c>
       <c r="N7" s="68" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="O7" s="65" t="s">
         <v>498</v>
@@ -4774,7 +4791,7 @@
         <v>502</v>
       </c>
       <c r="O13" s="68" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="P13" t="s">
         <v>288</v>
@@ -4852,7 +4869,7 @@
         <v>540</v>
       </c>
       <c r="O15" s="63" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -4891,7 +4908,7 @@
         <v>540</v>
       </c>
       <c r="O16" s="63" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -5035,10 +5052,10 @@
         <v>546</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="N20" s="63" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="O20" s="63" t="s">
         <v>442</v>
@@ -5083,10 +5100,10 @@
         <v>546</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="N21" s="63" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="O21" s="63" t="s">
         <v>442</v>
@@ -5125,7 +5142,7 @@
         <v>392</v>
       </c>
       <c r="O22" s="65" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -5161,7 +5178,7 @@
         <v>434</v>
       </c>
       <c r="N23" s="65" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -5197,7 +5214,7 @@
         <v>390</v>
       </c>
       <c r="N24" s="65" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -5233,7 +5250,7 @@
         <v>271</v>
       </c>
       <c r="K26" s="64" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="L26" s="55" t="s">
         <v>519</v>
@@ -5242,7 +5259,7 @@
         <v>442</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="O26" s="64" t="s">
         <v>508</v>
@@ -5281,13 +5298,13 @@
         <v>257</v>
       </c>
       <c r="K27" s="64" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="M27" s="64" t="s">
         <v>520</v>
       </c>
       <c r="O27" s="63" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -5440,10 +5457,10 @@
         <v>520</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="N31" s="64" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -5482,7 +5499,7 @@
         <v>520</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="M32" s="64" t="s">
         <v>522</v>
@@ -5521,7 +5538,7 @@
         <v>274</v>
       </c>
       <c r="K33" s="64" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L33" s="64" t="s">
         <v>520</v>
@@ -5563,10 +5580,10 @@
         <v>373</v>
       </c>
       <c r="K34" s="64" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="N34" s="68" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -5602,7 +5619,7 @@
         <v>352</v>
       </c>
       <c r="L35" s="64" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -5992,10 +6009,10 @@
         <v>555</v>
       </c>
       <c r="L46" s="64" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="M46" s="68" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="N46" s="64" t="s">
         <v>523</v>
@@ -6037,7 +6054,7 @@
         <v>555</v>
       </c>
       <c r="M47" s="68" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -6076,16 +6093,16 @@
         <v>555</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="M48" s="68" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="N48" s="68" t="s">
         <v>553</v>
       </c>
       <c r="O48" s="66" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
@@ -6268,7 +6285,7 @@
         <v>540</v>
       </c>
       <c r="O54" s="66" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -6346,7 +6363,7 @@
         <v>540</v>
       </c>
       <c r="O56" s="66" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -6541,7 +6558,7 @@
         <v>451</v>
       </c>
       <c r="K61" s="64" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="M61" s="65" t="s">
         <v>500</v>
@@ -6733,7 +6750,7 @@
         <v>456</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -6880,7 +6897,7 @@
         <v>400</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P71" t="s">
         <v>255</v>
@@ -6919,7 +6936,7 @@
         <v>313</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P72" t="s">
         <v>257</v>
@@ -7027,13 +7044,13 @@
         <v>367</v>
       </c>
       <c r="K75" s="69" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="N75" s="69" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="O75" s="67" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -7105,16 +7122,16 @@
         <v>328</v>
       </c>
       <c r="K77" s="69" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="L77" s="67" t="s">
         <v>517</v>
       </c>
       <c r="M77" s="68" t="s">
+        <v>589</v>
+      </c>
+      <c r="N77" s="4" t="s">
         <v>590</v>
-      </c>
-      <c r="N77" s="4" t="s">
-        <v>591</v>
       </c>
       <c r="P77" t="s">
         <v>299</v>
@@ -7156,7 +7173,7 @@
         <v>419</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="M78" s="64" t="s">
         <v>444</v>
@@ -7204,13 +7221,13 @@
         <v>519</v>
       </c>
       <c r="K79" s="67" t="s">
+        <v>577</v>
+      </c>
+      <c r="L79" s="70" t="s">
         <v>578</v>
       </c>
-      <c r="L79" s="70" t="s">
-        <v>579</v>
-      </c>
       <c r="M79" s="69" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="P79" t="s">
         <v>298</v>
@@ -7288,7 +7305,7 @@
         <v>428</v>
       </c>
       <c r="O81" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -7402,13 +7419,13 @@
         <v>367</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="N85" s="67" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="O85" s="68" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -7453,7 +7470,7 @@
         <v>521</v>
       </c>
       <c r="O86" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
@@ -7639,7 +7656,7 @@
         <v>517</v>
       </c>
       <c r="O91" s="67" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -7678,7 +7695,7 @@
         <v>502</v>
       </c>
       <c r="N92" s="68" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
@@ -7714,7 +7731,7 @@
         <v>318</v>
       </c>
       <c r="N94" s="67" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="O94" s="64" t="s">
         <v>512</v>
@@ -7753,19 +7770,19 @@
         <v>402</v>
       </c>
       <c r="K95" s="68" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="L95" s="69" t="s">
         <v>515</v>
       </c>
       <c r="M95" s="4" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N95" s="68" t="s">
         <v>502</v>
       </c>
       <c r="O95" s="69" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -7801,10 +7818,10 @@
         <v>415</v>
       </c>
       <c r="K96" s="69" t="s">
+        <v>580</v>
+      </c>
+      <c r="L96" s="4" t="s">
         <v>581</v>
-      </c>
-      <c r="L96" s="4" t="s">
-        <v>582</v>
       </c>
       <c r="M96" s="67" t="s">
         <v>517</v>
@@ -7852,10 +7869,10 @@
         <v>435</v>
       </c>
       <c r="K97" s="69" t="s">
+        <v>580</v>
+      </c>
+      <c r="L97" s="4" t="s">
         <v>581</v>
-      </c>
-      <c r="L97" s="4" t="s">
-        <v>582</v>
       </c>
       <c r="M97" s="67" t="s">
         <v>517</v>
@@ -7903,10 +7920,10 @@
         <v>435</v>
       </c>
       <c r="K98" s="69" t="s">
+        <v>580</v>
+      </c>
+      <c r="L98" s="4" t="s">
         <v>581</v>
-      </c>
-      <c r="L98" s="4" t="s">
-        <v>582</v>
       </c>
       <c r="M98" s="67" t="s">
         <v>517</v>
@@ -7993,7 +8010,7 @@
         <v>431</v>
       </c>
       <c r="K100" s="63" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
@@ -8077,7 +8094,7 @@
         <v>492</v>
       </c>
       <c r="N102" s="69" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
@@ -8113,7 +8130,7 @@
         <v>735</v>
       </c>
       <c r="K103" s="63" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
@@ -8266,7 +8283,7 @@
         <v>459</v>
       </c>
       <c r="N108" s="68" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
@@ -8398,7 +8415,7 @@
         <v>498</v>
       </c>
       <c r="O111" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
@@ -8437,7 +8454,7 @@
         <v>441</v>
       </c>
       <c r="O112" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
@@ -8988,7 +9005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -9095,67 +9112,67 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B19" s="54"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B20" s="54"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B21" s="54"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="54" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" s="54" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="54" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B25" s="54"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="54" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="54" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B28" s="54"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" s="54" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" s="54" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -9188,12 +9205,12 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -9218,23 +9235,23 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C50">
         <f>COUNTIF(Skills!J2:J122, "*")</f>
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D50">
         <f>COUNT(Skills!G2:G122)</f>
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F50" s="72" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G50" s="73"/>
     </row>
@@ -9244,14 +9261,14 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C52">
         <f>COUNTIF(Skills!$J$2:$J$122, "*damage*")</f>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F52" s="74" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="G52" s="75">
         <f>COUNTIF(Skills!$G$2:$G$122, "1")</f>
@@ -9260,30 +9277,30 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C53">
         <f>COUNTIF(Skills!$J$2:$J$122, "*heal*")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F53" s="74" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="G53" s="75">
         <f>COUNTIF(Skills!$G$2:$G$122, "2")</f>
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C54">
         <f>COUNTIF(Skills!$J$2:$J$122, "*shield*")</f>
         <v>7</v>
       </c>
       <c r="F54" s="74" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="G54" s="75">
         <f>COUNTIF(Skills!$G$2:$G$122, "3")</f>
@@ -9292,14 +9309,14 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C55">
         <f>COUNTIF(Skills!$J$2:$J$122, "* buff*")</f>
         <v>15</v>
       </c>
       <c r="F55" s="76" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="G55" s="77">
         <f>COUNTIF(Skills!$G$2:$G$122, "4")</f>
@@ -9308,7 +9325,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C56">
         <f>COUNTIF(Skills!$J$2:$J$122, "*debuff*")</f>
@@ -9317,7 +9334,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C57">
         <f>SUM(C58:C66)</f>
@@ -9326,7 +9343,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C58">
         <f>COUNTIF(Skills!$J$2:$J$122, "*bleed*")</f>
@@ -9341,7 +9358,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C59">
         <f>COUNTIF(Skills!$J$2:$J$122, "*stun*")</f>
@@ -9356,7 +9373,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C60">
         <f>COUNTIF(Skills!$J$2:$J$122, "*sleep*")</f>
@@ -9371,7 +9388,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B61" s="17"/>
       <c r="C61">
@@ -9387,7 +9404,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B62" s="17"/>
       <c r="C62">
@@ -9398,12 +9415,12 @@
         <v>15</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B63" s="17"/>
       <c r="C63">
@@ -9414,12 +9431,12 @@
         <v>15</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B64" s="17"/>
       <c r="C64">
@@ -9430,12 +9447,12 @@
         <v>10</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B65" s="17"/>
       <c r="C65">
@@ -9446,12 +9463,12 @@
         <v>40</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B66" s="17"/>
       <c r="C66">
@@ -9459,12 +9476,12 @@
         <v>3</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B67" s="17"/>
       <c r="C67">
@@ -9472,7 +9489,7 @@
         <v>2</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -9480,7 +9497,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C69">
         <f>COUNTIF(Skills!J134:J169, "**")</f>
@@ -9489,7 +9506,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C71">
         <f>COUNTIF(Skills!$J$134:$J$169, "*damage*")</f>
@@ -9498,7 +9515,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C72">
         <f>COUNTIF(Skills!$J$134:$J$169, "*immune*")</f>
@@ -9507,7 +9524,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C73">
         <f>COUNTIF(Skills!$J$134:$J$169, "*heal*")</f>
@@ -9516,7 +9533,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C74">
         <f>COUNTIF(Skills!$J$134:$J$169, "*shield*")</f>
@@ -9525,7 +9542,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C75">
         <f>COUNTIF(Skills!$J$134:$J$169, "* buff*")</f>
@@ -9534,7 +9551,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C76">
         <f>COUNTIF(Skills!$J$134:$J$169, "*debuff*")</f>
@@ -9543,7 +9560,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C77">
         <f>SUM(C78:C86)</f>
@@ -9552,7 +9569,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C78">
         <f>COUNTIF(Skills!$J$134:$J$169, "*bleed*")</f>
@@ -9561,7 +9578,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C79">
         <f>COUNTIF(Skills!$J$134:$J$169, "*stun*")</f>
@@ -9570,7 +9587,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C80">
         <f>COUNTIF(Skills!$J$134:$J$169, "*sleep*")</f>
@@ -9579,7 +9596,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C81">
         <f>COUNTIF(Skills!$J$134:$J$169, "*silence*")</f>
@@ -9588,7 +9605,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C82">
         <f>COUNTIF(Skills!$J$134:$J$169, "*burn*")</f>
@@ -9597,7 +9614,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C83">
         <f>COUNTIF(Skills!$J$134:$J$169, "*poison*")</f>
@@ -9606,7 +9623,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C84">
         <f>COUNTIF(Skills!$J$134:$J$169, "*bind*")</f>
@@ -9615,7 +9632,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C85">
         <f>COUNTIF(Skills!$J$134:$J$169, "*curse*")</f>
@@ -9624,7 +9641,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C86">
         <f>COUNTIF(Skills!$J$134:$J$169, "*energy*")</f>
@@ -9633,7 +9650,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -9641,7 +9658,7 @@
         <v>-10</v>
       </c>
       <c r="B89" s="78" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C89" s="37">
         <f>2/8</f>
@@ -9653,7 +9670,7 @@
         <v>-9</v>
       </c>
       <c r="B90" s="78" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C90" s="37">
         <f>1/3.75</f>
@@ -9665,7 +9682,7 @@
         <v>-8</v>
       </c>
       <c r="B91" s="78" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C91" s="37">
         <f>1/3.5</f>
@@ -9677,7 +9694,7 @@
         <v>-7</v>
       </c>
       <c r="B92" s="78" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C92" s="37">
         <f>1/3.25</f>
@@ -9689,7 +9706,7 @@
         <v>-6</v>
       </c>
       <c r="B93" s="78" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C93" s="37">
         <f>2/6</f>
@@ -9701,7 +9718,7 @@
         <v>-5</v>
       </c>
       <c r="B94" s="78" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C94" s="37">
         <f>1/2.75</f>
@@ -9713,7 +9730,7 @@
         <v>-4</v>
       </c>
       <c r="B95" s="78" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C95" s="37">
         <f>1/2.5</f>
@@ -9725,7 +9742,7 @@
         <v>-3</v>
       </c>
       <c r="B96" s="78" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C96" s="37">
         <f>1/2.25</f>
@@ -9737,7 +9754,7 @@
         <v>-2</v>
       </c>
       <c r="B97" s="78" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C97" s="37">
         <f>1/2</f>
@@ -9749,7 +9766,7 @@
         <v>-1</v>
       </c>
       <c r="B98" s="78" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C98" s="37">
         <f>1/1.5</f>
@@ -9761,7 +9778,7 @@
         <v>0</v>
       </c>
       <c r="B99" s="78" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C99" s="37">
         <v>1</v>
@@ -9772,7 +9789,7 @@
         <v>1</v>
       </c>
       <c r="B100" s="78" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C100" s="37">
         <v>1.5</v>
@@ -9783,7 +9800,7 @@
         <v>2</v>
       </c>
       <c r="B101" s="78" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C101" s="37">
         <v>2</v>
@@ -9794,7 +9811,7 @@
         <v>3</v>
       </c>
       <c r="B102" s="78" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C102" s="37">
         <v>2.25</v>
@@ -9805,7 +9822,7 @@
         <v>4</v>
       </c>
       <c r="B103" s="78" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C103" s="37">
         <v>2.5</v>
@@ -9816,7 +9833,7 @@
         <v>5</v>
       </c>
       <c r="B104" s="78" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C104" s="37">
         <v>2.75</v>
@@ -9827,7 +9844,7 @@
         <v>6</v>
       </c>
       <c r="B105" s="78" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C105" s="37">
         <v>3</v>
@@ -9838,7 +9855,7 @@
         <v>7</v>
       </c>
       <c r="B106" s="78" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C106" s="37">
         <v>3.25</v>
@@ -9849,7 +9866,7 @@
         <v>8</v>
       </c>
       <c r="B107" s="78" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C107" s="37">
         <v>3.5</v>
@@ -9860,7 +9877,7 @@
         <v>9</v>
       </c>
       <c r="B108" s="78" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C108" s="37">
         <v>3.75</v>
@@ -9871,7 +9888,7 @@
         <v>10</v>
       </c>
       <c r="B109" s="78" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C109" s="37">
         <v>4</v>
@@ -9885,11 +9902,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N190"/>
+  <dimension ref="A1:N194"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9923,13 +9940,13 @@
         <v>160</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H1" s="51" t="s">
+        <v>833</v>
+      </c>
+      <c r="I1" s="51" t="s">
         <v>834</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>835</v>
       </c>
       <c r="J1" s="50" t="s">
         <v>164</v>
@@ -9965,7 +9982,7 @@
         <v>55</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -9995,12 +10012,12 @@
         <v>60</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="63" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>438</v>
@@ -10025,12 +10042,12 @@
         <v>70</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="63" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>438</v>
@@ -10055,7 +10072,7 @@
         <v>45</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -10085,15 +10102,15 @@
         <v>65</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="63" t="s">
+        <v>775</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>776</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>777</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>0</v>
@@ -10115,7 +10132,7 @@
         <v>50</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -10123,7 +10140,7 @@
         <v>474</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>11</v>
@@ -10145,7 +10162,7 @@
         <v>70</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -10175,15 +10192,15 @@
         <v>40</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="63" t="s">
+        <v>759</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>760</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>761</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>438</v>
@@ -10205,15 +10222,15 @@
         <v>50</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="63" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>0</v>
@@ -10235,7 +10252,7 @@
         <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -10265,12 +10282,12 @@
         <v>45</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="63" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>477</v>
@@ -10295,7 +10312,7 @@
         <v>55</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -10303,7 +10320,7 @@
         <v>536</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>0</v>
@@ -10312,7 +10329,7 @@
         <v>30</v>
       </c>
       <c r="F14" s="49" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G14" s="49">
         <v>2</v>
@@ -10325,15 +10342,15 @@
         <v>67.5</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="63" t="s">
+        <v>751</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>752</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>753</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>0</v>
@@ -10342,7 +10359,7 @@
         <v>25</v>
       </c>
       <c r="F15" s="49" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G15" s="49">
         <v>2</v>
@@ -10355,15 +10372,15 @@
         <v>25</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="63" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>438</v>
@@ -10385,15 +10402,15 @@
         <v>20</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="63" t="s">
+        <v>654</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>655</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>656</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>438</v>
@@ -10415,15 +10432,15 @@
         <v>30</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="63" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>0</v>
@@ -10445,15 +10462,15 @@
         <v>45</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="63" t="s">
+        <v>828</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>829</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>830</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>0</v>
@@ -10462,7 +10479,7 @@
         <v>40</v>
       </c>
       <c r="F19" s="49" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G19" s="49">
         <v>2</v>
@@ -10475,15 +10492,15 @@
         <v>80</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="63" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>438</v>
@@ -10505,7 +10522,7 @@
         <v>22.5</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -10513,7 +10530,7 @@
         <v>505</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>0</v>
@@ -10535,12 +10552,12 @@
         <v>41.666666666666664</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="63" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>110</v>
@@ -10565,21 +10582,21 @@
         <v>40</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="63" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E23" s="49" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F23" s="49">
         <v>1</v>
@@ -10592,21 +10609,21 @@
         <v>#VALUE!</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="63" t="s">
+        <v>615</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>616</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>617</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F24" s="49">
         <v>1</v>
@@ -10619,7 +10636,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -10627,7 +10644,7 @@
         <v>504</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>438</v>
@@ -10649,15 +10666,15 @@
         <v>31.666666666666668</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="63" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>438</v>
@@ -10676,7 +10693,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -10684,7 +10701,7 @@
         <v>115</v>
       </c>
       <c r="B27" s="64" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>438</v>
@@ -10709,7 +10726,7 @@
         <v>50</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -10740,16 +10757,16 @@
         <v>65</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="57"/>
       <c r="B29" s="64" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>438</v>
@@ -10758,7 +10775,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="49" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="G29" s="49">
         <v>1</v>
@@ -10771,16 +10788,16 @@
         <v>40</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="57"/>
       <c r="B30" s="64" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>0</v>
@@ -10802,7 +10819,7 @@
         <v>40</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -10811,7 +10828,7 @@
         <v>508</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>0</v>
@@ -10833,7 +10850,7 @@
         <v>42.5</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -10842,7 +10859,7 @@
         <v>520</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>0</v>
@@ -10864,7 +10881,7 @@
         <v>40</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -10895,13 +10912,13 @@
         <v>60</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="57"/>
       <c r="B34" s="64" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>110</v>
@@ -10926,16 +10943,16 @@
         <v>42.5</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="57"/>
       <c r="B35" s="64" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>0</v>
@@ -10957,16 +10974,16 @@
         <v>60</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="57"/>
       <c r="B36" s="64" t="s">
+        <v>633</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>634</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>635</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>0</v>
@@ -10988,16 +11005,16 @@
         <v>45</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="57"/>
       <c r="B37" s="64" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>0</v>
@@ -11019,16 +11036,16 @@
         <v>40</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="57"/>
       <c r="B38" s="64" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>11</v>
@@ -11050,7 +11067,7 @@
         <v>45</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -11059,7 +11076,7 @@
         <v>444</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>438</v>
@@ -11081,16 +11098,16 @@
         <v>60</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="57"/>
       <c r="B40" s="64" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>438</v>
@@ -11112,7 +11129,7 @@
         <v>35</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -11121,7 +11138,7 @@
         <v>437</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>438</v>
@@ -11143,7 +11160,7 @@
         <v>50</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -11152,7 +11169,7 @@
         <v>512</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>11</v>
@@ -11174,16 +11191,16 @@
         <v>43.333333333333336</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="57"/>
       <c r="B43" s="64" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>11</v>
@@ -11205,7 +11222,7 @@
         <v>56.666666666666664</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -11214,7 +11231,7 @@
         <v>529</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>438</v>
@@ -11236,7 +11253,7 @@
         <v>53.333333333333336</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -11267,7 +11284,7 @@
         <v>40</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -11275,10 +11292,10 @@
         <v>188</v>
       </c>
       <c r="B46" s="65" t="s">
+        <v>744</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>745</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>746</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>438</v>
@@ -11297,7 +11314,7 @@
         <v>10</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -11306,7 +11323,7 @@
         <v>506</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>0</v>
@@ -11315,7 +11332,7 @@
         <v>20</v>
       </c>
       <c r="F47" s="49" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G47" s="49">
         <v>1</v>
@@ -11328,7 +11345,7 @@
         <v>100</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="K47" s="17"/>
     </row>
@@ -11361,7 +11378,7 @@
         <v>67.5</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -11370,7 +11387,7 @@
         <v>497</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>0</v>
@@ -11392,7 +11409,7 @@
         <v>40</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -11401,7 +11418,7 @@
         <v>500</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>11</v>
@@ -11423,17 +11440,17 @@
         <v>40</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="K50" s="17"/>
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="58"/>
       <c r="B51" s="65" t="s">
+        <v>626</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>627</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>628</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>0</v>
@@ -11455,7 +11472,7 @@
         <v>50</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -11472,7 +11489,7 @@
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="58"/>
       <c r="B53" s="65" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="I53" s="49" t="e">
         <f t="shared" si="0"/>
@@ -11486,7 +11503,7 @@
         <v>537</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>11</v>
@@ -11508,17 +11525,17 @@
         <v>40</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="K54" s="17"/>
     </row>
     <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="58"/>
       <c r="B55" s="65" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>0</v>
@@ -11540,17 +11557,17 @@
         <v>47.5</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="K55" s="17"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="58"/>
       <c r="B56" s="65" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>0</v>
@@ -11572,16 +11589,16 @@
         <v>50</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="58"/>
       <c r="B57" s="65" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>438</v>
@@ -11603,7 +11620,7 @@
         <v>73.333333333333329</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="K57" s="17"/>
     </row>
@@ -11613,7 +11630,7 @@
         <v>419</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>438</v>
@@ -11636,16 +11653,16 @@
         <v>40</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="58"/>
       <c r="B59" s="65" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>438</v>
@@ -11668,16 +11685,16 @@
         <v>66.666666666666671</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="58"/>
       <c r="B60" s="65" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>0</v>
@@ -11699,16 +11716,16 @@
         <v>41.666666666666664</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="58"/>
       <c r="B61" s="65" t="s">
+        <v>594</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>595</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>596</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>0</v>
@@ -11730,7 +11747,7 @@
         <v>42.5</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -11738,7 +11755,7 @@
         <v>189</v>
       </c>
       <c r="B62" s="67" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>438</v>
@@ -11763,7 +11780,7 @@
         <v>55</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -11794,7 +11811,7 @@
         <v>45</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -11825,16 +11842,16 @@
         <v>40</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="59"/>
       <c r="B65" s="67" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>438</v>
@@ -11843,7 +11860,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="49" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G65" s="49">
         <v>1</v>
@@ -11857,7 +11874,7 @@
         <v>80</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -11889,7 +11906,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -11898,7 +11915,7 @@
         <v>501</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>11</v>
@@ -11920,16 +11937,16 @@
         <v>40</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="59"/>
       <c r="B68" s="67" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>0</v>
@@ -11951,7 +11968,7 @@
         <v>50</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -11967,7 +11984,7 @@
     <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="59"/>
       <c r="B70" s="67" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>544</v>
@@ -11993,16 +12010,16 @@
         <v>48.75</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="59"/>
       <c r="B71" s="67" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>0</v>
@@ -12024,13 +12041,13 @@
         <v>47.5</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="59"/>
       <c r="B72" s="67" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>11</v>
@@ -12043,10 +12060,10 @@
     <row r="73" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="59"/>
       <c r="B73" s="67" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>11</v>
@@ -12065,16 +12082,16 @@
         <v>30</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="59"/>
       <c r="B74" s="67" t="s">
+        <v>782</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>783</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>784</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>11</v>
@@ -12083,7 +12100,7 @@
         <v>30</v>
       </c>
       <c r="F74" s="49" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G74" s="49">
         <v>2</v>
@@ -12097,16 +12114,16 @@
         <v>80</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="59"/>
       <c r="B75" s="67" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>0</v>
@@ -12128,16 +12145,16 @@
         <v>40</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="59"/>
       <c r="B76" s="67" t="s">
+        <v>572</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>573</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>574</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>0</v>
@@ -12159,7 +12176,7 @@
         <v>41.666666666666664</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -12168,7 +12185,7 @@
         <v>480</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>11</v>
@@ -12177,7 +12194,7 @@
         <v>40</v>
       </c>
       <c r="F77" s="49" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G77" s="49">
         <v>3</v>
@@ -12190,16 +12207,16 @@
         <v>70</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="59"/>
       <c r="B78" s="67" t="s">
+        <v>792</v>
+      </c>
+      <c r="C78" s="5" t="s">
         <v>793</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>794</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>11</v>
@@ -12221,7 +12238,7 @@
         <v>42.5</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -12229,10 +12246,10 @@
         <v>187</v>
       </c>
       <c r="B79" s="68" t="s">
+        <v>643</v>
+      </c>
+      <c r="C79" s="5" t="s">
         <v>644</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>645</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>438</v>
@@ -12254,7 +12271,7 @@
         <v>40</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -12263,7 +12280,7 @@
         <v>502</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>11</v>
@@ -12286,7 +12303,7 @@
         <v>62</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
@@ -12295,7 +12312,7 @@
         <v>510</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>11</v>
@@ -12317,16 +12334,16 @@
         <v>52.5</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="60"/>
       <c r="B82" s="68" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>0</v>
@@ -12348,7 +12365,7 @@
         <v>52.5</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -12379,13 +12396,13 @@
         <v>47.5</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="60"/>
       <c r="B84" s="68" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>554</v>
@@ -12410,16 +12427,16 @@
         <v>47.5</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="60"/>
       <c r="B85" s="68" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>11</v>
@@ -12441,16 +12458,16 @@
         <v>55</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="60"/>
       <c r="B86" s="68" t="s">
+        <v>623</v>
+      </c>
+      <c r="C86" s="5" t="s">
         <v>624</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>625</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>438</v>
@@ -12472,16 +12489,16 @@
         <v>45</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="60"/>
       <c r="B87" s="68" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>438</v>
@@ -12490,7 +12507,7 @@
         <v>0</v>
       </c>
       <c r="F87" s="49" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G87" s="49">
         <v>2</v>
@@ -12503,16 +12520,16 @@
         <v>20</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="60"/>
       <c r="B88" s="68" t="s">
+        <v>649</v>
+      </c>
+      <c r="C88" s="5" t="s">
         <v>650</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>651</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>438</v>
@@ -12534,7 +12551,7 @@
         <v>25</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -12543,7 +12560,7 @@
         <v>521</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>11</v>
@@ -12565,16 +12582,16 @@
         <v>43.333333333333336</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="60"/>
       <c r="B90" s="68" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>11</v>
@@ -12596,16 +12613,16 @@
         <v>40</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="60"/>
       <c r="B91" s="68" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>11</v>
@@ -12627,13 +12644,13 @@
         <v>41.666666666666664</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="60"/>
       <c r="B92" s="68" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>544</v>
@@ -12659,23 +12676,44 @@
         <v>50</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="60"/>
       <c r="B93" s="68" t="s">
         <v>543</v>
       </c>
-      <c r="I93" s="49" t="e">
+      <c r="C93" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" s="49">
+        <v>45</v>
+      </c>
+      <c r="F93" s="49">
+        <v>2</v>
+      </c>
+      <c r="G93" s="49">
+        <v>2</v>
+      </c>
+      <c r="H93" s="49">
+        <v>50</v>
+      </c>
+      <c r="I93" s="49">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>52.5</v>
+      </c>
+      <c r="J93" s="4" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="60"/>
       <c r="B94" s="68" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I94" s="49" t="e">
         <f t="shared" si="1"/>
@@ -12687,7 +12725,7 @@
         <v>186</v>
       </c>
       <c r="B95" s="69" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>438</v>
@@ -12712,7 +12750,7 @@
         <v>50</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
@@ -12743,7 +12781,7 @@
         <v>35</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
@@ -12774,16 +12812,16 @@
         <v>45</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="61"/>
       <c r="B98" s="69" t="s">
+        <v>823</v>
+      </c>
+      <c r="C98" s="5" t="s">
         <v>824</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>825</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>438</v>
@@ -12792,7 +12830,7 @@
         <v>0</v>
       </c>
       <c r="F98" s="49" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="G98" s="49">
         <v>1</v>
@@ -12805,16 +12843,16 @@
         <v>30</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="61"/>
       <c r="B99" s="69" t="s">
+        <v>830</v>
+      </c>
+      <c r="C99" s="5" t="s">
         <v>831</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>832</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>0</v>
@@ -12836,7 +12874,7 @@
         <v>40</v>
       </c>
       <c r="J99" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
@@ -12867,7 +12905,7 @@
         <v>45</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -12876,7 +12914,7 @@
         <v>513</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>0</v>
@@ -12898,7 +12936,7 @@
         <v>40</v>
       </c>
       <c r="J101" s="4" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
@@ -12907,7 +12945,7 @@
         <v>515</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>0</v>
@@ -12929,16 +12967,16 @@
         <v>55</v>
       </c>
       <c r="J102" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="61"/>
       <c r="B103" s="69" t="s">
+        <v>574</v>
+      </c>
+      <c r="C103" s="5" t="s">
         <v>575</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>576</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>11</v>
@@ -12960,16 +12998,16 @@
         <v>50</v>
       </c>
       <c r="J103" s="4" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="61"/>
       <c r="B104" s="69" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>11</v>
@@ -12991,22 +13029,22 @@
         <v>52.5</v>
       </c>
       <c r="J104" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="61"/>
       <c r="B105" s="69" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E105" s="49" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F105" s="49">
         <v>1</v>
@@ -13019,16 +13057,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="J105" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="61"/>
       <c r="B106" s="69" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>11</v>
@@ -13050,16 +13088,16 @@
         <v>40</v>
       </c>
       <c r="J106" s="4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="61"/>
       <c r="B107" s="69" t="s">
+        <v>636</v>
+      </c>
+      <c r="C107" s="5" t="s">
         <v>637</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>638</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>11</v>
@@ -13081,16 +13119,16 @@
         <v>50</v>
       </c>
       <c r="J107" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="61"/>
       <c r="B108" s="69" t="s">
+        <v>706</v>
+      </c>
+      <c r="C108" s="5" t="s">
         <v>707</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>708</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>0</v>
@@ -13112,16 +13150,16 @@
         <v>43.333333333333336</v>
       </c>
       <c r="J108" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="61"/>
       <c r="B109" s="69" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>11</v>
@@ -13130,7 +13168,7 @@
         <v>0</v>
       </c>
       <c r="F109" s="49" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G109" s="49">
         <v>3</v>
@@ -13144,16 +13182,16 @@
         <v>140</v>
       </c>
       <c r="J109" s="4" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A110" s="61"/>
       <c r="B110" s="69" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>438</v>
@@ -13162,7 +13200,7 @@
         <v>0</v>
       </c>
       <c r="F110" s="49" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G110" s="49">
         <v>3</v>
@@ -13175,16 +13213,16 @@
         <v>60</v>
       </c>
       <c r="J110" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="111" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="61"/>
       <c r="B111" s="69" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>11</v>
@@ -13193,7 +13231,7 @@
         <v>90</v>
       </c>
       <c r="F111" s="49" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G111" s="49">
         <v>4</v>
@@ -13206,7 +13244,7 @@
         <v>67.5</v>
       </c>
       <c r="J111" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
@@ -13239,7 +13277,7 @@
         <v>65</v>
       </c>
       <c r="J112" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
@@ -13270,16 +13308,16 @@
         <v>45</v>
       </c>
       <c r="J113" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="62"/>
       <c r="B114" s="66" t="s">
+        <v>630</v>
+      </c>
+      <c r="C114" s="5" t="s">
         <v>631</v>
-      </c>
-      <c r="C114" s="5" t="s">
-        <v>632</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>11</v>
@@ -13288,7 +13326,7 @@
         <v>40</v>
       </c>
       <c r="F114" s="49" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G114" s="49">
         <v>2</v>
@@ -13302,7 +13340,7 @@
         <v>80</v>
       </c>
       <c r="J114" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -13311,7 +13349,7 @@
         <v>511</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>11</v>
@@ -13333,7 +13371,7 @@
         <v>40</v>
       </c>
       <c r="J115" s="4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -13364,16 +13402,16 @@
         <v>40</v>
       </c>
       <c r="J116" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="62"/>
       <c r="B117" s="66" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>11</v>
@@ -13395,7 +13433,7 @@
         <v>42.5</v>
       </c>
       <c r="J117" s="4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -13426,16 +13464,16 @@
         <v>50</v>
       </c>
       <c r="J118" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="62"/>
       <c r="B119" s="66" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>11</v>
@@ -13457,7 +13495,7 @@
         <v>57.5</v>
       </c>
       <c r="J119" s="4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
@@ -13467,10 +13505,10 @@
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="62"/>
       <c r="B121" s="66" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>0</v>
@@ -13492,16 +13530,16 @@
         <v>48.333333333333336</v>
       </c>
       <c r="J121" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="62"/>
       <c r="B122" s="66" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>0</v>
@@ -13523,16 +13561,16 @@
         <v>40</v>
       </c>
       <c r="J122" s="4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="62"/>
       <c r="B123" s="66" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>11</v>
@@ -13554,16 +13592,16 @@
         <v>63.333333333333336</v>
       </c>
       <c r="J123" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="124" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="62"/>
       <c r="B124" s="66" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>0</v>
@@ -13572,7 +13610,7 @@
         <v>40</v>
       </c>
       <c r="F124" s="49" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G124" s="49">
         <v>4</v>
@@ -13586,13 +13624,13 @@
         <v>84</v>
       </c>
       <c r="J124" s="4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="125" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="62"/>
       <c r="B125" s="66" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C125" s="5" t="s">
         <v>496</v>
@@ -13604,7 +13642,7 @@
         <v>80</v>
       </c>
       <c r="F125" s="49" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G125" s="49">
         <v>4</v>
@@ -13617,19 +13655,19 @@
         <v>60</v>
       </c>
       <c r="J125" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="62"/>
       <c r="B126" s="66" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="62"/>
       <c r="B127" s="66" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>438</v>
@@ -13648,7 +13686,7 @@
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="62"/>
       <c r="B128" s="66" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I128" s="49" t="e">
         <f t="shared" si="1"/>
@@ -13672,10 +13710,10 @@
         <v>479</v>
       </c>
       <c r="E134" s="49" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="J134" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="N134" s="54"/>
     </row>
@@ -13687,13 +13725,13 @@
         <v>557</v>
       </c>
       <c r="J135" s="4" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="N135" s="54"/>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B136" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="N136" s="54"/>
     </row>
@@ -13711,19 +13749,19 @@
         <v>556</v>
       </c>
       <c r="J138" s="4" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="N138" s="54"/>
     </row>
-    <row r="139" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="B139" s="4" t="s">
         <v>558</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>560</v>
+        <v>897</v>
       </c>
       <c r="J139" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N139" s="54"/>
     </row>
@@ -13732,148 +13770,148 @@
         <v>559</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="J140" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N140" s="54"/>
     </row>
     <row r="141" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B141" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="C141" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="C141" s="5" t="s">
-        <v>564</v>
-      </c>
       <c r="J141" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="N141" s="54"/>
     </row>
     <row r="142" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B142" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="J142" s="4" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="N142" s="54"/>
     </row>
     <row r="143" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B143" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="C143" s="5" t="s">
         <v>583</v>
       </c>
-      <c r="C143" s="5" t="s">
-        <v>584</v>
-      </c>
       <c r="J143" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N143" s="54"/>
     </row>
     <row r="144" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J144" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="N144" s="54"/>
     </row>
     <row r="145" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="B145" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J145" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="N145" s="54"/>
     </row>
     <row r="146" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="B146" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="C146" s="5" t="s">
         <v>597</v>
       </c>
-      <c r="C146" s="5" t="s">
-        <v>598</v>
-      </c>
       <c r="J146" s="4" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="N146" s="54"/>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B147" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="N147" s="54"/>
     </row>
     <row r="148" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B148" s="4" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C148" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="J148" s="4" t="s">
         <v>802</v>
-      </c>
-      <c r="J148" s="4" t="s">
-        <v>803</v>
       </c>
       <c r="N148" s="54"/>
     </row>
     <row r="149" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B149" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="C149" s="5" t="s">
         <v>640</v>
       </c>
-      <c r="C149" s="5" t="s">
-        <v>641</v>
-      </c>
       <c r="J149" s="4" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="N149" s="54"/>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B150" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="C150" s="5" t="s">
         <v>653</v>
       </c>
-      <c r="C150" s="5" t="s">
-        <v>654</v>
-      </c>
       <c r="J150" s="4" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="N150" s="54"/>
     </row>
     <row r="151" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B151" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="C151" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="C151" s="5" t="s">
-        <v>689</v>
-      </c>
       <c r="J151" s="4" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="N151" s="54"/>
     </row>
     <row r="152" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B152" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="C152" s="5" t="s">
         <v>697</v>
       </c>
-      <c r="C152" s="5" t="s">
-        <v>698</v>
-      </c>
       <c r="J152" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="N152" s="54"/>
     </row>
@@ -13883,17 +13921,17 @@
         <v>519</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="J153" s="4" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="N153" s="54"/>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="71"/>
       <c r="B154" s="70" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="N154" s="54"/>
     </row>
@@ -13910,10 +13948,10 @@
         <v>542</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J156" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N156" s="54"/>
     </row>
@@ -13923,10 +13961,10 @@
         <v>441</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="J157" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.25">
@@ -13940,23 +13978,23 @@
         <v>503</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="J159" s="4" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="N159" s="54"/>
     </row>
     <row r="160" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="71"/>
       <c r="B160" s="70" t="s">
+        <v>765</v>
+      </c>
+      <c r="C160" s="5" t="s">
         <v>766</v>
       </c>
-      <c r="C160" s="5" t="s">
-        <v>767</v>
-      </c>
       <c r="J160" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N160" s="54"/>
     </row>
@@ -13966,10 +14004,10 @@
         <v>527</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="J161" s="4" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="N161" s="54"/>
     </row>
@@ -13979,36 +14017,36 @@
         <v>516</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="J162" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="N162" s="54"/>
     </row>
     <row r="163" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="71"/>
       <c r="B163" s="70" t="s">
+        <v>772</v>
+      </c>
+      <c r="C163" s="5" t="s">
         <v>773</v>
       </c>
-      <c r="C163" s="5" t="s">
-        <v>774</v>
-      </c>
       <c r="J163" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N163" s="54"/>
     </row>
     <row r="164" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="71"/>
       <c r="B164" s="70" t="s">
+        <v>578</v>
+      </c>
+      <c r="C164" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="C164" s="5" t="s">
-        <v>580</v>
-      </c>
       <c r="J164" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N164" s="54"/>
     </row>
@@ -14018,10 +14056,10 @@
         <v>440</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="J165" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N165" s="54"/>
     </row>
@@ -14031,10 +14069,10 @@
         <v>514</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="J166" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="N166" s="54"/>
     </row>
@@ -14044,10 +14082,10 @@
         <v>518</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="J167" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="N167" s="54"/>
     </row>
@@ -14060,240 +14098,266 @@
     </row>
     <row r="169" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="B169" s="4" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="J169" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A170" s="50" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A171" s="4" t="s">
-        <v>130</v>
-      </c>
+      <c r="B170" s="4" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="B171" s="4" t="s">
-        <v>446</v>
+        <v>892</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>106</v>
+        <v>893</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B172" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="C172" s="5" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B173" s="4" t="s">
-        <v>448</v>
+        <v>896</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>435</v>
+        <v>898</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B174" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="C174" s="5" t="s">
-        <v>433</v>
+      <c r="A174" s="50" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A175" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="B175" s="4" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>436</v>
+        <v>106</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B176" s="4" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B177" s="4" t="s">
-        <v>607</v>
+        <v>448</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>609</v>
+        <v>435</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B178" s="4" t="s">
-        <v>608</v>
+        <v>449</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>610</v>
+        <v>433</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B179" s="4" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B180" s="4" t="s">
-        <v>569</v>
+        <v>451</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B181" s="4" t="s">
-        <v>570</v>
+        <v>606</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B182" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="C182" s="5" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B183" s="4" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B184" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="C184" s="5" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B185" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="C185" s="5" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B186" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="C186" s="5" t="s">
         <v>605</v>
       </c>
-      <c r="C182" s="5" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" s="57" t="s">
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="B183" s="64" t="s">
+      <c r="B187" s="64" t="s">
         <v>484</v>
       </c>
-      <c r="D183" s="6" t="s">
+      <c r="D187" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E183" s="49">
+      <c r="E187" s="49">
         <v>135</v>
       </c>
-      <c r="G183" s="49">
+      <c r="G187" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A184" s="57"/>
-      <c r="B184" s="64" t="s">
+    <row r="188" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A188" s="57"/>
+      <c r="B188" s="64" t="s">
         <v>549</v>
       </c>
-      <c r="C184" s="5" t="s">
+      <c r="C188" s="5" t="s">
         <v>548</v>
-      </c>
-      <c r="D184" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E184" s="49">
-        <v>25</v>
-      </c>
-      <c r="G184" s="49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A185" s="58" t="s">
-        <v>188</v>
-      </c>
-      <c r="B185" s="63" t="s">
-        <v>483</v>
-      </c>
-      <c r="C185" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="D185" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E185" s="49">
-        <v>120</v>
-      </c>
-      <c r="G185" s="49">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A186" s="59" t="s">
-        <v>189</v>
-      </c>
-      <c r="B186" s="63" t="s">
-        <v>485</v>
-      </c>
-      <c r="D186" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E186" s="49">
-        <v>140</v>
-      </c>
-      <c r="G186" s="49">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" s="60"/>
-      <c r="B187" s="63" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" s="60" t="s">
-        <v>187</v>
-      </c>
-      <c r="B188" s="63" t="s">
-        <v>482</v>
       </c>
       <c r="D188" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E188" s="49">
-        <v>135</v>
+        <v>25</v>
       </c>
       <c r="G188" s="49">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A189" s="61" t="s">
-        <v>186</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A189" s="58" t="s">
+        <v>188</v>
       </c>
       <c r="B189" s="63" t="s">
-        <v>481</v>
+        <v>483</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>420</v>
       </c>
       <c r="D189" s="6" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E189" s="49">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="G189" s="49">
         <v>4</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A190" s="62" t="s">
+      <c r="A190" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="B190" s="63" t="s">
+        <v>485</v>
+      </c>
+      <c r="D190" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E190" s="49">
+        <v>140</v>
+      </c>
+      <c r="G190" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191" s="60"/>
+      <c r="B191" s="63" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="B192" s="63" t="s">
+        <v>482</v>
+      </c>
+      <c r="D192" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E192" s="49">
+        <v>135</v>
+      </c>
+      <c r="G192" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193" s="61" t="s">
+        <v>186</v>
+      </c>
+      <c r="B193" s="63" t="s">
+        <v>481</v>
+      </c>
+      <c r="D193" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E193" s="49">
+        <v>140</v>
+      </c>
+      <c r="G193" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="B190" s="63"/>
-      <c r="D190" s="6" t="s">
+      <c r="B194" s="63"/>
+      <c r="D194" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E190" s="49">
+      <c r="E194" s="49">
         <v>135</v>
       </c>
-      <c r="G190" s="49">
+      <c r="G194" s="49">
         <v>4</v>
       </c>
     </row>
@@ -14308,8 +14372,8 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15199,13 +15263,13 @@
         <v>9</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C46" s="8">
         <v>2</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>11</v>
@@ -15219,7 +15283,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>14</v>
@@ -15345,7 +15409,7 @@
         <v>184</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C54" s="8">
         <v>1</v>
@@ -15365,7 +15429,7 @@
         <v>184</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C55" s="8">
         <v>1</v>
@@ -15409,7 +15473,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>0</v>
@@ -15690,7 +15754,7 @@
         <v>1</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C77" s="8">
         <v>1</v>
@@ -15900,7 +15964,7 @@
         <v>2</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>11</v>
@@ -15920,13 +15984,13 @@
     </row>
     <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="12" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C99" s="8">
         <v>2</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>11</v>
@@ -16152,7 +16216,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -16162,32 +16226,32 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -16195,12 +16259,12 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>